<commit_message>
added code for test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="132" yWindow="540" windowWidth="22716" windowHeight="10788"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="512">
   <si>
     <t>ID</t>
   </si>
@@ -406,9 +406,6 @@
     <t>IRCTC_TC_23</t>
   </si>
   <si>
-    <t>div[class='ng-star-inserted']:nth-of-type(1)&gt;div[class*='form-group']:nth-of-type(1)&gt;app-train-avl-enq&gt;div[class='ng-star-inserted']:nth-of-type(1)&gt;div[class*='white-back']:nth-of-type(3)&gt;div[class*='col-xs-']:nth-of-type(1)</t>
-  </si>
-  <si>
     <t>//div[@class='ng-star-inserted'][1]/div[contains(@class, 'form-group')][1]//div[contains(@class, 'white-back')]/div[contains(@class, 'col-xs-')][1]</t>
   </si>
   <si>
@@ -481,9 +478,6 @@
     <t>INDORE_NIC_04</t>
   </si>
   <si>
-    <t>div[class='copyRightsText'] p:nth-of-type(2)</t>
-  </si>
-  <si>
     <t>//div[@class='copyRightsText']/p[2]</t>
   </si>
   <si>
@@ -499,15 +493,9 @@
     <t>https://indore.nic.in/en/agriculture/</t>
   </si>
   <si>
-    <t>tr:nth-of-type(1) td[data-th='OFFICER']</t>
-  </si>
-  <si>
     <t>//tr[1]/td[@data-th='OFFICER']</t>
   </si>
   <si>
-    <t>tr td[data-th='OFFICER']</t>
-  </si>
-  <si>
     <t>//tr/td[@data-th='OFFICER']</t>
   </si>
   <si>
@@ -535,18 +523,6 @@
     <t>https://indore.nic.in/en/document-category/master-plan-20-21/</t>
   </si>
   <si>
-    <t>tr:nth-of-type(1) td[data-th='Title '] span[class='bt-content']</t>
-  </si>
-  <si>
-    <t>//tr[1]/td[@data-th='Title ']/span[@class='bt-content']</t>
-  </si>
-  <si>
-    <t>tr td[data-th='Title '] span[class='bt-content']</t>
-  </si>
-  <si>
-    <t>//tr/td[@data-th='Title ']/span[@class='bt-content']</t>
-  </si>
-  <si>
     <t>span:contains(Master Plan 20-21- Studies and Analysis Part – 3)</t>
   </si>
   <si>
@@ -595,15 +571,9 @@
     <t>INDORE_NIC_10</t>
   </si>
   <si>
-    <t>div[id*='post-'] p:nth-of-type(2)</t>
-  </si>
-  <si>
     <t>//div[contains(@id, 'post-')]/p[2]</t>
   </si>
   <si>
-    <t>div[id*='post-'] p</t>
-  </si>
-  <si>
     <t>//div[contains(@id, 'post-')]/p</t>
   </si>
   <si>
@@ -634,9 +604,6 @@
     <t>https://yonobusiness.sbi/</t>
   </si>
   <si>
-    <t>a[rel='external'] img</t>
-  </si>
-  <si>
     <t>//a[@rel='external']/img</t>
   </si>
   <si>
@@ -733,9 +700,6 @@
     <t>YONO_SBI_07</t>
   </si>
   <si>
-    <t>div[class='float-right hidden-xs'] p</t>
-  </si>
-  <si>
     <t>//div[@class='float-right hidden-xs']/p</t>
   </si>
   <si>
@@ -1340,13 +1304,259 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>div[class='ng-star-inserted']:nth-of-type(1)&gt;div[class*='form-group']:nth-of-type(1) div[class*='white-back']:nth-of-type(3)&gt;div[class*='col-xs-']:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>div[class='copyRightsText'] &gt; p:nth-of-type(2)</t>
+  </si>
+  <si>
+    <t>tr:nth-of-type(1) &gt; td[data-th='OFFICER']</t>
+  </si>
+  <si>
+    <t>tr &gt; td[data-th='OFFICER']</t>
+  </si>
+  <si>
+    <t>tr:nth-of-type(1) &gt; td[data-th*='Title'] &gt; span[class='bt-content']</t>
+  </si>
+  <si>
+    <t>//tr[1]/td[contains(@data-th, 'Title')]/span[@class='bt-content']</t>
+  </si>
+  <si>
+    <t>tr &gt; td[data-th*='Title'] &gt; span[class='bt-content']</t>
+  </si>
+  <si>
+    <t>//tr/td[contains(@data-th, 'Title')]/span[@class='bt-content']</t>
+  </si>
+  <si>
+    <t>div[id*='post-'] &gt; p:nth-of-type(2)</t>
+  </si>
+  <si>
+    <t>div[id*='post-'] &gt; p</t>
+  </si>
+  <si>
+    <t>a[rel='external'] &gt; img</t>
+  </si>
+  <si>
+    <t>div[class='float-right hidden-xs'] &gt; p</t>
+  </si>
+  <si>
+    <t>JOY_BIRD_06</t>
+  </si>
+  <si>
+    <t>https://joybird.com/</t>
+  </si>
+  <si>
+    <t>svg[class='sc-DJfgX jNGuMj']</t>
+  </si>
+  <si>
+    <t>//*[name()='svg'][@class='sc-DJfgX jNGuMj']</t>
+  </si>
+  <si>
+    <t>iframe[scrolling='no']</t>
+  </si>
+  <si>
+    <t>//iframe[@scrolling='no']</t>
+  </si>
+  <si>
+    <t>Shubham</t>
+  </si>
+  <si>
+    <t>UITRGPV_AC_09</t>
+  </si>
+  <si>
+    <t>div[class*='col-lg-']:nth-of-type(1) div[class='footer_col'] ul[class='list-item']&gt;i[class='la la-angle-right']:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>//footer//div[contains(@class, 'col-lg-')][1]//ul[@class='list-item']/i[@class='la la-angle-right'][1]</t>
+  </si>
+  <si>
+    <t>div[class*='col-lg-'] div[class='footer_col'] ul[class='list-item']&gt;i[class='la la-angle-right']</t>
+  </si>
+  <si>
+    <t>//footer//div[contains(@class, 'col-lg-')]//ul[@class='list-item']/i[@class='la la-angle-right']</t>
+  </si>
+  <si>
+    <t>kapil</t>
+  </si>
+  <si>
+    <t>Demo_QA_04</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/select-menu</t>
+  </si>
+  <si>
+    <t>div[class='row']:nth-of-type(7)&gt;div[class*='col-md-']&gt;div[class*='css-']&gt;div[class*='css-']:nth-of-type(1)&gt;div[class*='css-']:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>//div[@class='row'][2]/div[contains(@class, 'col-md-')]/div[contains(@class, 'css-')]/div[contains(@class, 'css-')][1]/div[contains(@class, 'css-')][1]</t>
+  </si>
+  <si>
+    <t>div[class='row']&gt;div[class*='col-md-']&gt;div[class*='css-']&gt;div[class*='css-']&gt;div[class*='css-']</t>
+  </si>
+  <si>
+    <t>//div[@class='row']/div[contains(@class, 'col-md-')]/div[contains(@class, 'css-')]/div[contains(@class, 'css-')]/div[contains(@class, 'css-')]</t>
+  </si>
+  <si>
+    <t>div:contains(Select...)</t>
+  </si>
+  <si>
+    <t>//div[contains(text(), 'Select...')]</t>
+  </si>
+  <si>
+    <t>Demo_QA_05</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/menu#</t>
+  </si>
+  <si>
+    <t>ul[id='nav']&gt;li:nth-of-type(1)&gt;a</t>
+  </si>
+  <si>
+    <t>//ul[@id='nav']/li[1]/a</t>
+  </si>
+  <si>
+    <t>ul[id='nav']&gt;li&gt;a</t>
+  </si>
+  <si>
+    <t>//ul[@id='nav']/li/a</t>
+  </si>
+  <si>
+    <t>a:contains(Main Item 1)</t>
+  </si>
+  <si>
+    <t>//a[contains(text(), 'Main Item 1')]</t>
+  </si>
+  <si>
+    <t>Freshers_Jobs_02</t>
+  </si>
+  <si>
+    <t>h4 font[color*='ff'] font</t>
+  </si>
+  <si>
+    <t>//h4[6]/font[contains(@color, 'ff')]/font</t>
+  </si>
+  <si>
+    <t>//h4/font[contains(@color, 'ff')]/font</t>
+  </si>
+  <si>
+    <t>font:contains(Fresher Jobs – FAQs:)</t>
+  </si>
+  <si>
+    <t>//font[contains(text(), 'Fresher Jobs – FAQs:')]</t>
+  </si>
+  <si>
+    <t>Freshers_Jobs_03</t>
+  </si>
+  <si>
+    <t>div[id*='footer']:nth-of-type(1)&gt;div[class='footer-column section']&gt;div[id*='HTML']&gt;div[class='widget-content']</t>
+  </si>
+  <si>
+    <t>//div[@id='footer-column-container']/div[contains(@id, 'footer')][1]//ul/li[1]</t>
+  </si>
+  <si>
+    <t>div[id*='footer']&gt;div[class='footer-column section']&gt;div[id*='HTML']&gt;div[class='widget-content']</t>
+  </si>
+  <si>
+    <t>//div[@id='footer-column-container']/div[contains(@id, 'footer')]//ul/li</t>
+  </si>
+  <si>
+    <t>Free_Jobs_Alert_01</t>
+  </si>
+  <si>
+    <t>https://www.freejobalert.com/government-jobs/</t>
+  </si>
+  <si>
+    <t>input[id*='gsc-i-id']</t>
+  </si>
+  <si>
+    <t>//input[contains(@id, 'gsc-i-id')]</t>
+  </si>
+  <si>
+    <t>Free_Jobs_Alert_02</t>
+  </si>
+  <si>
+    <t>div[class*='gb-grid-column']:nth-of-type(1) ul li:nth-of-type(1) a</t>
+  </si>
+  <si>
+    <t>//div[contains(@class, 'gb-grid-column')][1]//ul/li[1]/a</t>
+  </si>
+  <si>
+    <t>div[class*='gb-grid-column'] ul li a</t>
+  </si>
+  <si>
+    <t>//div[contains(@class, 'gb-grid-column')]//ul/li/a</t>
+  </si>
+  <si>
+    <t>a:contains(Latest Notifications)</t>
+  </si>
+  <si>
+    <t>(//a[contains(text(), 'Latest Notifications')])[2]</t>
+  </si>
+  <si>
+    <t>Linkedin_01</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/</t>
+  </si>
+  <si>
+    <t>li[class*='global-nav']:nth-of-type(2) svg[class='mercado-match']</t>
+  </si>
+  <si>
+    <t>//li[contains(@class, 'global-nav')][2]//*[name()='svg'][@class='mercado-match']</t>
+  </si>
+  <si>
+    <t>li[class*='global-nav'] svg[class='mercado-match']</t>
+  </si>
+  <si>
+    <t>//li[contains(@class, 'global-nav')]//*[name()='svg'][@class='mercado-match']</t>
+  </si>
+  <si>
+    <t>Linkedin_02</t>
+  </si>
+  <si>
+    <t>div[class='share-box-feed-entry__top-bar'] &gt; button[class*='artdeco-button']</t>
+  </si>
+  <si>
+    <t>//div[@class='share-box-feed-entry__top-bar']/button[contains(@class, 'artdeco-button')]</t>
+  </si>
+  <si>
+    <t>Linkedin_03</t>
+  </si>
+  <si>
+    <t>div[class*='community-panel-inte']:nth-of-type(1) &gt; ul[class='community-panel-interest-package__section-expanded']&gt;li[class='community-panel-interest-package__entity-item truncate']:nth-of-type(1) span[class*='hashtag-a']:nth-of-type(2)</t>
+  </si>
+  <si>
+    <t>//div[contains(@class, 'community-panel-inte')][1]/ul[@class='community-panel-interest-package__section-expanded']//li[@class='community-panel-interest-package__entity-item truncate'][1]//span[contains(@class, 'hashtag-a')]//span[contains(@class, 'hashtag-a')]</t>
+  </si>
+  <si>
+    <t>div[class*='community-panel-inte'] &gt; ul[class='community-panel-interest-package__section-expanded']&gt;li[class='community-panel-interest-package__entity-item truncate'] span[class*='hashtag-a']</t>
+  </si>
+  <si>
+    <t>//div[contains(@class, 'community-panel-inte')]/ul[@class='community-panel-interest-package__section-expanded']//li[@class='community-panel-interest-package__entity-item truncate']//span[contains(@class, 'hashtag-a')]//span[contains(@class, 'hashtag-a')]</t>
+  </si>
+  <si>
+    <t>span:contains(jobseekers)</t>
+  </si>
+  <si>
+    <t>(//span[contains(text(), 'jobseekers')])[1]</t>
+  </si>
+  <si>
+    <t>Linkedin_04</t>
+  </si>
+  <si>
+    <t>p[class*='identity-headline']</t>
+  </si>
+  <si>
+    <t>//p[contains(@class, 'identity-headline')]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1383,6 +1593,26 @@
       <color rgb="FF333333"/>
       <name val="Body"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1398,7 +1628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1406,11 +1636,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1442,8 +1691,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1653,14 +1910,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1007"/>
+  <dimension ref="A1:AA1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1742,22 +1999,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>15</v>
@@ -1793,22 +2050,22 @@
         <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>15</v>
@@ -1850,10 +2107,10 @@
         <v>23</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>24</v>
@@ -1895,22 +2152,22 @@
         <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>15</v>
@@ -1946,16 +2203,16 @@
         <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>32</v>
@@ -2003,16 +2260,16 @@
         <v>39</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>40</v>
@@ -2054,16 +2311,16 @@
         <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>15</v>
@@ -2105,10 +2362,10 @@
         <v>50</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>51</v>
@@ -2156,10 +2413,10 @@
         <v>58</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>59</v>
@@ -2204,13 +2461,13 @@
         <v>64</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>65</v>
@@ -2252,22 +2509,22 @@
         <v>69</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>53</v>
@@ -2309,16 +2566,16 @@
         <v>74</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>53</v>
@@ -2360,10 +2617,10 @@
         <v>78</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>79</v>
@@ -2411,10 +2668,10 @@
         <v>85</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>86</v>
@@ -2462,10 +2719,10 @@
         <v>92</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>93</v>
@@ -2513,16 +2770,16 @@
         <v>99</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>88</v>
@@ -2558,22 +2815,22 @@
         <v>102</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>103</v>
@@ -2609,16 +2866,16 @@
         <v>106</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>107</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>108</v>
@@ -2653,11 +2910,11 @@
       <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="9" t="s">
         <v>111</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>112</v>
@@ -2666,10 +2923,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>114</v>
@@ -2711,22 +2968,22 @@
         <v>117</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>118</v>
@@ -2762,22 +3019,22 @@
         <v>120</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>121</v>
@@ -2819,10 +3076,10 @@
         <v>126</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>127</v>
@@ -2857,29 +3114,29 @@
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="G24" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>121</v>
@@ -2903,34 +3160,34 @@
     </row>
     <row r="25" spans="1:27">
       <c r="A25" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>121</v>
@@ -2954,34 +3211,34 @@
     </row>
     <row r="26" spans="1:27">
       <c r="A26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>121</v>
@@ -3005,34 +3262,34 @@
     </row>
     <row r="27" spans="1:27">
       <c r="A27" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="G27" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>121</v>
@@ -3056,34 +3313,34 @@
     </row>
     <row r="28" spans="1:27">
       <c r="A28" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="G28" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>121</v>
@@ -3107,34 +3364,34 @@
     </row>
     <row r="29" spans="1:27">
       <c r="A29" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="E29" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>164</v>
-      </c>
       <c r="G29" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>121</v>
@@ -3158,34 +3415,34 @@
     </row>
     <row r="30" spans="1:27">
       <c r="A30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="G30" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>121</v>
@@ -3209,34 +3466,34 @@
     </row>
     <row r="31" spans="1:27">
       <c r="A31" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>437</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>121</v>
@@ -3260,34 +3517,34 @@
     </row>
     <row r="32" spans="1:27">
       <c r="A32" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>121</v>
@@ -3311,34 +3568,34 @@
     </row>
     <row r="33" spans="1:27">
       <c r="A33" s="5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>188</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>121</v>
@@ -3362,34 +3619,34 @@
     </row>
     <row r="34" spans="1:27">
       <c r="A34" s="5" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>193</v>
+        <v>438</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>196</v>
+        <v>439</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>198</v>
+        <v>429</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>188</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>121</v>
@@ -3413,34 +3670,34 @@
     </row>
     <row r="35" spans="1:27">
       <c r="A35" s="5" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>121</v>
@@ -3464,34 +3721,34 @@
     </row>
     <row r="36" spans="1:27">
       <c r="A36" s="3" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>206</v>
+        <v>195</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>440</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>121</v>
@@ -3515,34 +3772,34 @@
     </row>
     <row r="37" spans="1:27">
       <c r="A37" s="3" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>121</v>
@@ -3566,34 +3823,34 @@
     </row>
     <row r="38" spans="1:27">
       <c r="A38" s="3" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="I38" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="J38" s="5" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>121</v>
@@ -3617,34 +3874,34 @@
     </row>
     <row r="39" spans="1:27">
       <c r="A39" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>121</v>
@@ -3668,34 +3925,34 @@
     </row>
     <row r="40" spans="1:27">
       <c r="A40" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>121</v>
@@ -3719,34 +3976,34 @@
     </row>
     <row r="41" spans="1:27">
       <c r="A41" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>121</v>
@@ -3770,34 +4027,34 @@
     </row>
     <row r="42" spans="1:27">
       <c r="A42" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>239</v>
+        <v>195</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>441</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>121</v>
@@ -3821,34 +4078,34 @@
     </row>
     <row r="43" spans="1:27">
       <c r="A43" s="3" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>121</v>
@@ -3872,34 +4129,34 @@
     </row>
     <row r="44" spans="1:27">
       <c r="A44" s="3" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>121</v>
@@ -3923,34 +4180,34 @@
     </row>
     <row r="45" spans="1:27">
       <c r="A45" s="3" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>121</v>
@@ -3974,34 +4231,34 @@
     </row>
     <row r="46" spans="1:27">
       <c r="A46" s="3" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>121</v>
@@ -4025,34 +4282,34 @@
     </row>
     <row r="47" spans="1:27">
       <c r="A47" s="3" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>121</v>
@@ -4076,34 +4333,34 @@
     </row>
     <row r="48" spans="1:27">
       <c r="A48" s="3" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>264</v>
-      </c>
       <c r="G48" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>121</v>
@@ -4125,36 +4382,36 @@
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>121</v>
@@ -4176,87 +4433,79 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
     </row>
-    <row r="50" spans="1:27">
-      <c r="A50" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="5"/>
-      <c r="U50" s="5"/>
-      <c r="V50" s="5"/>
-      <c r="W50" s="5"/>
-      <c r="X50" s="5"/>
-      <c r="Y50" s="5"/>
-      <c r="Z50" s="5"/>
-      <c r="AA50" s="5"/>
-    </row>
-    <row r="51" spans="1:27">
+    <row r="50" spans="1:27" ht="40.200000000000003" thickBot="1">
+      <c r="A50" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+      <c r="Y50" s="11"/>
+      <c r="Z50" s="11"/>
+      <c r="AA50" s="11"/>
+    </row>
+    <row r="51" spans="1:27" ht="79.2">
       <c r="A51" s="3" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K51" s="5" t="s">
         <v>121</v>
@@ -4280,34 +4529,34 @@
     </row>
     <row r="52" spans="1:27">
       <c r="A52" s="3" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>290</v>
+        <v>429</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>291</v>
+        <v>429</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>121</v>
@@ -4331,37 +4580,37 @@
     </row>
     <row r="53" spans="1:27">
       <c r="A53" s="3" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>294</v>
-      </c>
       <c r="E53" s="5" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>441</v>
+        <v>121</v>
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
@@ -4381,89 +4630,89 @@
       <c r="AA53" s="5"/>
     </row>
     <row r="54" spans="1:27">
-      <c r="A54" s="5" t="s">
-        <v>299</v>
+      <c r="A54" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>300</v>
+        <v>263</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
-      <c r="U54" s="9"/>
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
-      <c r="X54" s="9"/>
-      <c r="Y54" s="9"/>
-      <c r="Z54" s="9"/>
-      <c r="AA54" s="9"/>
+        <v>429</v>
+      </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="5"/>
     </row>
     <row r="55" spans="1:27">
       <c r="A55" s="5" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>441</v>
+        <v>290</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>292</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -4484,37 +4733,37 @@
     </row>
     <row r="56" spans="1:27">
       <c r="A56" s="5" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>318</v>
+        <v>298</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>121</v>
+        <v>295</v>
       </c>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
@@ -4535,34 +4784,34 @@
     </row>
     <row r="57" spans="1:27">
       <c r="A57" s="5" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="K57" s="5" t="s">
         <v>121</v>
@@ -4586,37 +4835,37 @@
     </row>
     <row r="58" spans="1:27">
       <c r="A58" s="5" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>307</v>
+        <v>121</v>
       </c>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
@@ -4637,37 +4886,37 @@
     </row>
     <row r="59" spans="1:27">
       <c r="A59" s="5" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>441</v>
+        <v>320</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>441</v>
+        <v>321</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>441</v>
+        <v>322</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>441</v>
+        <v>323</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
@@ -4688,37 +4937,37 @@
     </row>
     <row r="60" spans="1:27">
       <c r="A60" s="5" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>441</v>
+        <v>326</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>429</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I60" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="J60" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>429</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>121</v>
+        <v>295</v>
       </c>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -4739,37 +4988,37 @@
     </row>
     <row r="61" spans="1:27">
       <c r="A61" s="5" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>347</v>
+        <v>429</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>307</v>
+        <v>121</v>
       </c>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
@@ -4790,37 +5039,37 @@
     </row>
     <row r="62" spans="1:27">
       <c r="A62" s="5" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>351</v>
+        <v>334</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>354</v>
+        <v>429</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>121</v>
+        <v>295</v>
       </c>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
@@ -4841,34 +5090,34 @@
     </row>
     <row r="63" spans="1:27">
       <c r="A63" s="5" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>121</v>
@@ -4892,34 +5141,34 @@
     </row>
     <row r="64" spans="1:27">
       <c r="A64" s="5" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>363</v>
-      </c>
       <c r="D64" s="5" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="K64" s="5" t="s">
         <v>121</v>
@@ -4942,144 +5191,144 @@
       <c r="AA64" s="9"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>441</v>
+      <c r="A65" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>354</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>356</v>
       </c>
       <c r="K65" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L65" s="6"/>
-      <c r="M65" s="6"/>
-      <c r="N65" s="6"/>
-      <c r="O65" s="6"/>
-      <c r="P65" s="6"/>
-      <c r="Q65" s="6"/>
-      <c r="R65" s="6"/>
-      <c r="S65" s="6"/>
-      <c r="T65" s="6"/>
-      <c r="U65" s="6"/>
-      <c r="V65" s="6"/>
-      <c r="W65" s="6"/>
-      <c r="X65" s="6"/>
-      <c r="Y65" s="6"/>
-      <c r="Z65" s="6"/>
-      <c r="AA65" s="6"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="9"/>
+      <c r="S65" s="9"/>
+      <c r="T65" s="9"/>
+      <c r="U65" s="9"/>
+      <c r="V65" s="9"/>
+      <c r="W65" s="9"/>
+      <c r="X65" s="9"/>
+      <c r="Y65" s="9"/>
+      <c r="Z65" s="9"/>
+      <c r="AA65" s="9"/>
     </row>
     <row r="66" spans="1:27">
       <c r="A66" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>376</v>
+        <v>357</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>429</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I66" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="J66" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>429</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L66" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
-      <c r="O66" s="9"/>
-      <c r="P66" s="9"/>
-      <c r="Q66" s="9"/>
-      <c r="R66" s="9"/>
-      <c r="S66" s="9"/>
-      <c r="T66" s="9"/>
-      <c r="U66" s="9"/>
-      <c r="V66" s="9"/>
-      <c r="W66" s="9"/>
-      <c r="X66" s="9"/>
-      <c r="Y66" s="9"/>
-      <c r="Z66" s="9"/>
-      <c r="AA66" s="9"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
+      <c r="U66" s="6"/>
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="6"/>
+      <c r="Y66" s="6"/>
+      <c r="Z66" s="6"/>
+      <c r="AA66" s="6"/>
     </row>
     <row r="67" spans="1:27">
       <c r="A67" s="3" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L67" s="9"/>
+      <c r="L67" s="5" t="s">
+        <v>365</v>
+      </c>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
@@ -5098,34 +5347,34 @@
     </row>
     <row r="68" spans="1:27">
       <c r="A68" s="3" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="B68" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>387</v>
-      </c>
       <c r="G68" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>389</v>
+        <v>429</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="J68" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="K68" s="5" t="s">
         <v>121</v>
@@ -5149,92 +5398,90 @@
     </row>
     <row r="69" spans="1:27">
       <c r="A69" s="3" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>441</v>
+        <v>358</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>375</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I69" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>377</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
-      <c r="O69" s="6"/>
-      <c r="P69" s="6"/>
-      <c r="Q69" s="6"/>
-      <c r="R69" s="6"/>
-      <c r="S69" s="6"/>
-      <c r="T69" s="6"/>
-      <c r="U69" s="6"/>
-      <c r="V69" s="6"/>
-      <c r="W69" s="6"/>
-      <c r="X69" s="6"/>
-      <c r="Y69" s="6"/>
-      <c r="Z69" s="6"/>
-      <c r="AA69" s="6"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="9"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="9"/>
+      <c r="R69" s="9"/>
+      <c r="S69" s="9"/>
+      <c r="T69" s="9"/>
+      <c r="U69" s="9"/>
+      <c r="V69" s="9"/>
+      <c r="W69" s="9"/>
+      <c r="X69" s="9"/>
+      <c r="Y69" s="9"/>
+      <c r="Z69" s="9"/>
+      <c r="AA69" s="9"/>
     </row>
     <row r="70" spans="1:27">
       <c r="A70" s="3" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>397</v>
+        <v>358</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>429</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="K70" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L70" s="3" t="s">
-        <v>398</v>
-      </c>
+      <c r="L70" s="6"/>
       <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
@@ -5252,86 +5499,88 @@
       <c r="AA70" s="6"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="5" t="s">
-        <v>399</v>
+      <c r="A71" s="3" t="s">
+        <v>381</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>402</v>
+        <v>358</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>384</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>405</v>
+        <v>429</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>429</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L71" s="9"/>
-      <c r="M71" s="9"/>
-      <c r="N71" s="9"/>
-      <c r="O71" s="9"/>
-      <c r="P71" s="9"/>
-      <c r="Q71" s="9"/>
-      <c r="R71" s="9"/>
-      <c r="S71" s="9"/>
-      <c r="T71" s="9"/>
-      <c r="U71" s="9"/>
-      <c r="V71" s="9"/>
-      <c r="W71" s="9"/>
-      <c r="X71" s="9"/>
-      <c r="Y71" s="9"/>
-      <c r="Z71" s="9"/>
-      <c r="AA71" s="9"/>
+      <c r="L71" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="6"/>
+      <c r="T71" s="6"/>
+      <c r="U71" s="6"/>
+      <c r="V71" s="6"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="6"/>
+      <c r="Y71" s="6"/>
+      <c r="Z71" s="6"/>
+      <c r="AA71" s="6"/>
     </row>
     <row r="72" spans="1:27">
       <c r="A72" s="5" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>58</v>
+        <v>391</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="K72" s="5" t="s">
         <v>121</v>
@@ -5353,36 +5602,36 @@
       <c r="Z72" s="9"/>
       <c r="AA72" s="9"/>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" ht="106.2" thickBot="1">
       <c r="A73" s="5" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>413</v>
+        <v>358</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>417</v>
+        <v>58</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>418</v>
+        <v>398</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>419</v>
+        <v>399</v>
       </c>
       <c r="K73" s="5" t="s">
         <v>121</v>
@@ -5404,87 +5653,81 @@
       <c r="Z73" s="9"/>
       <c r="AA73" s="9"/>
     </row>
-    <row r="74" spans="1:27">
-      <c r="A74" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="H74" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="I74" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="J74" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="K74" s="5" t="s">
+    <row r="74" spans="1:27" ht="106.2" thickBot="1">
+      <c r="A74" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="11"/>
+      <c r="K74" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
-      <c r="N74" s="9"/>
-      <c r="O74" s="9"/>
-      <c r="P74" s="9"/>
-      <c r="Q74" s="9"/>
-      <c r="R74" s="9"/>
-      <c r="S74" s="9"/>
-      <c r="T74" s="9"/>
-      <c r="U74" s="9"/>
-      <c r="V74" s="9"/>
-      <c r="W74" s="9"/>
-      <c r="X74" s="9"/>
-      <c r="Y74" s="9"/>
-      <c r="Z74" s="9"/>
-      <c r="AA74" s="9"/>
-    </row>
-    <row r="75" spans="1:27">
+      <c r="L74" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M74" s="11"/>
+      <c r="N74" s="11"/>
+      <c r="O74" s="11"/>
+      <c r="P74" s="11"/>
+      <c r="Q74" s="11"/>
+      <c r="R74" s="11"/>
+      <c r="S74" s="11"/>
+      <c r="T74" s="11"/>
+      <c r="U74" s="11"/>
+      <c r="V74" s="11"/>
+      <c r="W74" s="11"/>
+      <c r="X74" s="11"/>
+      <c r="Y74" s="11"/>
+      <c r="Z74" s="11"/>
+      <c r="AA74" s="11"/>
+    </row>
+    <row r="75" spans="1:27" ht="118.8">
       <c r="A75" s="5" t="s">
-        <v>428</v>
+        <v>400</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="C75" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="G75" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>441</v>
-      </c>
       <c r="H75" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>431</v>
+        <v>406</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>432</v>
+        <v>407</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>121</v>
@@ -5508,34 +5751,34 @@
     </row>
     <row r="76" spans="1:27">
       <c r="A76" s="5" t="s">
-        <v>433</v>
+        <v>408</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>434</v>
+        <v>409</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>435</v>
+        <v>410</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>436</v>
+        <v>411</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>437</v>
+        <v>412</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>438</v>
+        <v>413</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>439</v>
+        <v>414</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>440</v>
+        <v>415</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>121</v>
@@ -5557,355 +5800,557 @@
       <c r="Z76" s="9"/>
       <c r="AA76" s="9"/>
     </row>
-    <row r="77" spans="1:27">
-      <c r="A77" s="6"/>
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
-      <c r="M77" s="6"/>
-      <c r="N77" s="6"/>
-      <c r="O77" s="6"/>
-      <c r="P77" s="6"/>
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
-      <c r="S77" s="6"/>
-      <c r="T77" s="6"/>
-      <c r="U77" s="6"/>
-      <c r="V77" s="6"/>
-      <c r="W77" s="6"/>
-      <c r="X77" s="6"/>
-      <c r="Y77" s="6"/>
-      <c r="Z77" s="6"/>
-      <c r="AA77" s="6"/>
-    </row>
-    <row r="78" spans="1:27">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6"/>
-      <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
-      <c r="S78" s="6"/>
-      <c r="T78" s="6"/>
-      <c r="U78" s="6"/>
-      <c r="V78" s="6"/>
-      <c r="W78" s="6"/>
-      <c r="X78" s="6"/>
-      <c r="Y78" s="6"/>
-      <c r="Z78" s="6"/>
-      <c r="AA78" s="6"/>
-    </row>
-    <row r="79" spans="1:27">
-      <c r="A79" s="6"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-      <c r="N79" s="6"/>
-      <c r="O79" s="6"/>
-      <c r="P79" s="6"/>
-      <c r="Q79" s="6"/>
-      <c r="R79" s="6"/>
-      <c r="S79" s="6"/>
-      <c r="T79" s="6"/>
-      <c r="U79" s="6"/>
-      <c r="V79" s="6"/>
-      <c r="W79" s="6"/>
-      <c r="X79" s="6"/>
-      <c r="Y79" s="6"/>
-      <c r="Z79" s="6"/>
-      <c r="AA79" s="6"/>
-    </row>
-    <row r="80" spans="1:27">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="6"/>
-      <c r="P80" s="6"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="6"/>
-      <c r="S80" s="6"/>
-      <c r="T80" s="6"/>
-      <c r="U80" s="6"/>
-      <c r="V80" s="6"/>
-      <c r="W80" s="6"/>
-      <c r="X80" s="6"/>
-      <c r="Y80" s="6"/>
-      <c r="Z80" s="6"/>
-      <c r="AA80" s="6"/>
-    </row>
-    <row r="81" spans="1:27">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="6"/>
-      <c r="M81" s="6"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="6"/>
-      <c r="P81" s="6"/>
-      <c r="Q81" s="6"/>
-      <c r="R81" s="6"/>
-      <c r="S81" s="6"/>
-      <c r="T81" s="6"/>
-      <c r="U81" s="6"/>
-      <c r="V81" s="6"/>
-      <c r="W81" s="6"/>
-      <c r="X81" s="6"/>
-      <c r="Y81" s="6"/>
-      <c r="Z81" s="6"/>
-      <c r="AA81" s="6"/>
-    </row>
-    <row r="82" spans="1:27">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
-      <c r="H82" s="6"/>
-      <c r="I82" s="6"/>
-      <c r="J82" s="6"/>
-      <c r="K82" s="6"/>
-      <c r="L82" s="6"/>
-      <c r="M82" s="6"/>
-      <c r="N82" s="6"/>
-      <c r="O82" s="6"/>
-      <c r="P82" s="6"/>
-      <c r="Q82" s="6"/>
-      <c r="R82" s="6"/>
-      <c r="S82" s="6"/>
-      <c r="T82" s="6"/>
-      <c r="U82" s="6"/>
-      <c r="V82" s="6"/>
-      <c r="W82" s="6"/>
-      <c r="X82" s="6"/>
-      <c r="Y82" s="6"/>
-      <c r="Z82" s="6"/>
-      <c r="AA82" s="6"/>
-    </row>
-    <row r="83" spans="1:27">
-      <c r="A83" s="6"/>
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
-      <c r="H83" s="6"/>
-      <c r="I83" s="6"/>
-      <c r="J83" s="6"/>
-      <c r="K83" s="6"/>
-      <c r="L83" s="6"/>
-      <c r="M83" s="6"/>
-      <c r="N83" s="6"/>
-      <c r="O83" s="6"/>
-      <c r="P83" s="6"/>
-      <c r="Q83" s="6"/>
-      <c r="R83" s="6"/>
-      <c r="S83" s="6"/>
-      <c r="T83" s="6"/>
-      <c r="U83" s="6"/>
-      <c r="V83" s="6"/>
-      <c r="W83" s="6"/>
-      <c r="X83" s="6"/>
-      <c r="Y83" s="6"/>
-      <c r="Z83" s="6"/>
-      <c r="AA83" s="6"/>
-    </row>
-    <row r="84" spans="1:27">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-      <c r="J84" s="6"/>
-      <c r="K84" s="6"/>
-      <c r="L84" s="6"/>
-      <c r="M84" s="6"/>
-      <c r="N84" s="6"/>
-      <c r="O84" s="6"/>
-      <c r="P84" s="6"/>
-      <c r="Q84" s="6"/>
-      <c r="R84" s="6"/>
-      <c r="S84" s="6"/>
-      <c r="T84" s="6"/>
-      <c r="U84" s="6"/>
-      <c r="V84" s="6"/>
-      <c r="W84" s="6"/>
-      <c r="X84" s="6"/>
-      <c r="Y84" s="6"/>
-      <c r="Z84" s="6"/>
-      <c r="AA84" s="6"/>
-    </row>
-    <row r="85" spans="1:27">
-      <c r="A85" s="6"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
-      <c r="H85" s="6"/>
-      <c r="I85" s="6"/>
-      <c r="J85" s="6"/>
-      <c r="K85" s="6"/>
-      <c r="L85" s="6"/>
-      <c r="M85" s="6"/>
-      <c r="N85" s="6"/>
-      <c r="O85" s="6"/>
-      <c r="P85" s="6"/>
-      <c r="Q85" s="6"/>
-      <c r="R85" s="6"/>
-      <c r="S85" s="6"/>
-      <c r="T85" s="6"/>
-      <c r="U85" s="6"/>
-      <c r="V85" s="6"/>
-      <c r="W85" s="6"/>
-      <c r="X85" s="6"/>
-      <c r="Y85" s="6"/>
-      <c r="Z85" s="6"/>
-      <c r="AA85" s="6"/>
-    </row>
-    <row r="86" spans="1:27">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="6"/>
-      <c r="I86" s="6"/>
-      <c r="J86" s="6"/>
-      <c r="K86" s="6"/>
-      <c r="L86" s="6"/>
-      <c r="M86" s="6"/>
-      <c r="N86" s="6"/>
-      <c r="O86" s="6"/>
-      <c r="P86" s="6"/>
-      <c r="Q86" s="6"/>
-      <c r="R86" s="6"/>
-      <c r="S86" s="6"/>
-      <c r="T86" s="6"/>
-      <c r="U86" s="6"/>
-      <c r="V86" s="6"/>
-      <c r="W86" s="6"/>
-      <c r="X86" s="6"/>
-      <c r="Y86" s="6"/>
-      <c r="Z86" s="6"/>
-      <c r="AA86" s="6"/>
-    </row>
-    <row r="87" spans="1:27">
-      <c r="A87" s="6"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="6"/>
-      <c r="M87" s="6"/>
-      <c r="N87" s="6"/>
-      <c r="O87" s="6"/>
-      <c r="P87" s="6"/>
-      <c r="Q87" s="6"/>
-      <c r="R87" s="6"/>
-      <c r="S87" s="6"/>
-      <c r="T87" s="6"/>
-      <c r="U87" s="6"/>
-      <c r="V87" s="6"/>
-      <c r="W87" s="6"/>
-      <c r="X87" s="6"/>
-      <c r="Y87" s="6"/>
-      <c r="Z87" s="6"/>
-      <c r="AA87" s="6"/>
-    </row>
-    <row r="88" spans="1:27">
-      <c r="A88" s="6"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6"/>
-      <c r="H88" s="6"/>
-      <c r="I88" s="6"/>
-      <c r="J88" s="6"/>
-      <c r="K88" s="6"/>
-      <c r="L88" s="6"/>
-      <c r="M88" s="6"/>
-      <c r="N88" s="6"/>
-      <c r="O88" s="6"/>
-      <c r="P88" s="6"/>
-      <c r="Q88" s="6"/>
-      <c r="R88" s="6"/>
-      <c r="S88" s="6"/>
-      <c r="T88" s="6"/>
-      <c r="U88" s="6"/>
-      <c r="V88" s="6"/>
-      <c r="W88" s="6"/>
-      <c r="X88" s="6"/>
-      <c r="Y88" s="6"/>
-      <c r="Z88" s="6"/>
-      <c r="AA88" s="6"/>
-    </row>
-    <row r="89" spans="1:27">
+    <row r="77" spans="1:27" ht="40.200000000000003" thickBot="1">
+      <c r="A77" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+      <c r="O77" s="9"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="9"/>
+      <c r="R77" s="9"/>
+      <c r="S77" s="9"/>
+      <c r="T77" s="9"/>
+      <c r="U77" s="9"/>
+      <c r="V77" s="9"/>
+      <c r="W77" s="9"/>
+      <c r="X77" s="9"/>
+      <c r="Y77" s="9"/>
+      <c r="Z77" s="9"/>
+      <c r="AA77" s="9"/>
+    </row>
+    <row r="78" spans="1:27" ht="145.80000000000001" thickBot="1">
+      <c r="A78" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="J78" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="K78" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L78" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M78" s="11"/>
+      <c r="N78" s="11"/>
+      <c r="O78" s="11"/>
+      <c r="P78" s="11"/>
+      <c r="Q78" s="11"/>
+      <c r="R78" s="11"/>
+      <c r="S78" s="11"/>
+      <c r="T78" s="11"/>
+      <c r="U78" s="11"/>
+      <c r="V78" s="11"/>
+      <c r="W78" s="11"/>
+      <c r="X78" s="11"/>
+      <c r="Y78" s="11"/>
+      <c r="Z78" s="11"/>
+      <c r="AA78" s="11"/>
+    </row>
+    <row r="79" spans="1:27" ht="27" thickBot="1">
+      <c r="A79" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="J79" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="K79" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L79" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M79" s="11"/>
+      <c r="N79" s="11"/>
+      <c r="O79" s="11"/>
+      <c r="P79" s="11"/>
+      <c r="Q79" s="11"/>
+      <c r="R79" s="11"/>
+      <c r="S79" s="11"/>
+      <c r="T79" s="11"/>
+      <c r="U79" s="11"/>
+      <c r="V79" s="11"/>
+      <c r="W79" s="11"/>
+      <c r="X79" s="11"/>
+      <c r="Y79" s="11"/>
+      <c r="Z79" s="11"/>
+      <c r="AA79" s="11"/>
+    </row>
+    <row r="80" spans="1:27" ht="66.599999999999994" thickBot="1">
+      <c r="A80" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L80" s="9"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
+      <c r="O80" s="9"/>
+      <c r="P80" s="9"/>
+      <c r="Q80" s="9"/>
+      <c r="R80" s="9"/>
+      <c r="S80" s="9"/>
+      <c r="T80" s="9"/>
+      <c r="U80" s="9"/>
+      <c r="V80" s="9"/>
+      <c r="W80" s="9"/>
+      <c r="X80" s="9"/>
+      <c r="Y80" s="9"/>
+      <c r="Z80" s="9"/>
+      <c r="AA80" s="9"/>
+    </row>
+    <row r="81" spans="1:27" ht="40.200000000000003" thickBot="1">
+      <c r="A81" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="E81" s="11"/>
+      <c r="F81" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="J81" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="K81" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L81" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M81" s="11"/>
+      <c r="N81" s="11"/>
+      <c r="O81" s="11"/>
+      <c r="P81" s="11"/>
+      <c r="Q81" s="11"/>
+      <c r="R81" s="11"/>
+      <c r="S81" s="11"/>
+      <c r="T81" s="11"/>
+      <c r="U81" s="11"/>
+      <c r="V81" s="11"/>
+      <c r="W81" s="11"/>
+      <c r="X81" s="11"/>
+      <c r="Y81" s="11"/>
+      <c r="Z81" s="11"/>
+      <c r="AA81" s="11"/>
+    </row>
+    <row r="82" spans="1:27" ht="79.8" thickBot="1">
+      <c r="A82" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="F82" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="11"/>
+      <c r="K82" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L82" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M82" s="11"/>
+      <c r="N82" s="11"/>
+      <c r="O82" s="11"/>
+      <c r="P82" s="11"/>
+      <c r="Q82" s="11"/>
+      <c r="R82" s="11"/>
+      <c r="S82" s="11"/>
+      <c r="T82" s="11"/>
+      <c r="U82" s="11"/>
+      <c r="V82" s="11"/>
+      <c r="W82" s="11"/>
+      <c r="X82" s="11"/>
+      <c r="Y82" s="11"/>
+      <c r="Z82" s="11"/>
+      <c r="AA82" s="11"/>
+    </row>
+    <row r="83" spans="1:27" ht="27" thickBot="1">
+      <c r="A83" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="L83" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M83" s="11"/>
+      <c r="N83" s="11"/>
+      <c r="O83" s="11"/>
+      <c r="P83" s="11"/>
+      <c r="Q83" s="11"/>
+      <c r="R83" s="11"/>
+      <c r="S83" s="11"/>
+      <c r="T83" s="11"/>
+      <c r="U83" s="11"/>
+      <c r="V83" s="11"/>
+      <c r="W83" s="11"/>
+      <c r="X83" s="11"/>
+      <c r="Y83" s="11"/>
+      <c r="Z83" s="11"/>
+      <c r="AA83" s="11"/>
+    </row>
+    <row r="84" spans="1:27" ht="66.599999999999994" thickBot="1">
+      <c r="A84" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="J84" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="K84" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L84" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M84" s="11"/>
+      <c r="N84" s="11"/>
+      <c r="O84" s="11"/>
+      <c r="P84" s="11"/>
+      <c r="Q84" s="11"/>
+      <c r="R84" s="11"/>
+      <c r="S84" s="11"/>
+      <c r="T84" s="11"/>
+      <c r="U84" s="11"/>
+      <c r="V84" s="11"/>
+      <c r="W84" s="11"/>
+      <c r="X84" s="11"/>
+      <c r="Y84" s="11"/>
+      <c r="Z84" s="11"/>
+      <c r="AA84" s="11"/>
+    </row>
+    <row r="85" spans="1:27" ht="79.8" thickBot="1">
+      <c r="A85" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+      <c r="L85" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M85" s="11"/>
+      <c r="N85" s="11"/>
+      <c r="O85" s="11"/>
+      <c r="P85" s="11"/>
+      <c r="Q85" s="11"/>
+      <c r="R85" s="11"/>
+      <c r="S85" s="11"/>
+      <c r="T85" s="11"/>
+      <c r="U85" s="11"/>
+      <c r="V85" s="11"/>
+      <c r="W85" s="11"/>
+      <c r="X85" s="11"/>
+      <c r="Y85" s="11"/>
+      <c r="Z85" s="11"/>
+      <c r="AA85" s="11"/>
+    </row>
+    <row r="86" spans="1:27" ht="93" thickBot="1">
+      <c r="A86" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="11"/>
+      <c r="K86" s="11"/>
+      <c r="L86" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M86" s="11"/>
+      <c r="N86" s="11"/>
+      <c r="O86" s="11"/>
+      <c r="P86" s="11"/>
+      <c r="Q86" s="11"/>
+      <c r="R86" s="11"/>
+      <c r="S86" s="11"/>
+      <c r="T86" s="11"/>
+      <c r="U86" s="11"/>
+      <c r="V86" s="11"/>
+      <c r="W86" s="11"/>
+      <c r="X86" s="11"/>
+      <c r="Y86" s="11"/>
+      <c r="Z86" s="11"/>
+      <c r="AA86" s="11"/>
+    </row>
+    <row r="87" spans="1:27" ht="277.8" thickBot="1">
+      <c r="A87" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="J87" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="K87" s="11"/>
+      <c r="L87" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M87" s="11"/>
+      <c r="N87" s="11"/>
+      <c r="O87" s="11"/>
+      <c r="P87" s="11"/>
+      <c r="Q87" s="11"/>
+      <c r="R87" s="11"/>
+      <c r="S87" s="11"/>
+      <c r="T87" s="11"/>
+      <c r="U87" s="11"/>
+      <c r="V87" s="11"/>
+      <c r="W87" s="11"/>
+      <c r="X87" s="11"/>
+      <c r="Y87" s="11"/>
+      <c r="Z87" s="11"/>
+      <c r="AA87" s="11"/>
+    </row>
+    <row r="88" spans="1:27" ht="27" thickBot="1">
+      <c r="A88" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
+      <c r="K88" s="11"/>
+      <c r="L88" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="M88" s="11"/>
+      <c r="N88" s="11"/>
+      <c r="O88" s="11"/>
+      <c r="P88" s="11"/>
+      <c r="Q88" s="11"/>
+      <c r="R88" s="11"/>
+      <c r="S88" s="11"/>
+      <c r="T88" s="11"/>
+      <c r="U88" s="11"/>
+      <c r="V88" s="11"/>
+      <c r="W88" s="11"/>
+      <c r="X88" s="11"/>
+      <c r="Y88" s="11"/>
+      <c r="Z88" s="11"/>
+      <c r="AA88" s="11"/>
+    </row>
+    <row r="89" spans="1:27" ht="13.2">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -32555,6 +33000,93 @@
       <c r="Y1007" s="6"/>
       <c r="Z1007" s="6"/>
       <c r="AA1007" s="6"/>
+    </row>
+    <row r="1008" spans="1:27">
+      <c r="A1008" s="6"/>
+      <c r="B1008" s="6"/>
+      <c r="C1008" s="6"/>
+      <c r="D1008" s="6"/>
+      <c r="E1008" s="6"/>
+      <c r="F1008" s="6"/>
+      <c r="G1008" s="6"/>
+      <c r="H1008" s="6"/>
+      <c r="I1008" s="6"/>
+      <c r="J1008" s="6"/>
+      <c r="K1008" s="6"/>
+      <c r="L1008" s="6"/>
+      <c r="M1008" s="6"/>
+      <c r="N1008" s="6"/>
+      <c r="O1008" s="6"/>
+      <c r="P1008" s="6"/>
+      <c r="Q1008" s="6"/>
+      <c r="R1008" s="6"/>
+      <c r="S1008" s="6"/>
+      <c r="T1008" s="6"/>
+      <c r="U1008" s="6"/>
+      <c r="V1008" s="6"/>
+      <c r="W1008" s="6"/>
+      <c r="X1008" s="6"/>
+      <c r="Y1008" s="6"/>
+      <c r="Z1008" s="6"/>
+      <c r="AA1008" s="6"/>
+    </row>
+    <row r="1009" spans="1:27">
+      <c r="A1009" s="6"/>
+      <c r="B1009" s="6"/>
+      <c r="C1009" s="6"/>
+      <c r="D1009" s="6"/>
+      <c r="E1009" s="6"/>
+      <c r="F1009" s="6"/>
+      <c r="G1009" s="6"/>
+      <c r="H1009" s="6"/>
+      <c r="I1009" s="6"/>
+      <c r="J1009" s="6"/>
+      <c r="K1009" s="6"/>
+      <c r="L1009" s="6"/>
+      <c r="M1009" s="6"/>
+      <c r="N1009" s="6"/>
+      <c r="O1009" s="6"/>
+      <c r="P1009" s="6"/>
+      <c r="Q1009" s="6"/>
+      <c r="R1009" s="6"/>
+      <c r="S1009" s="6"/>
+      <c r="T1009" s="6"/>
+      <c r="U1009" s="6"/>
+      <c r="V1009" s="6"/>
+      <c r="W1009" s="6"/>
+      <c r="X1009" s="6"/>
+      <c r="Y1009" s="6"/>
+      <c r="Z1009" s="6"/>
+      <c r="AA1009" s="6"/>
+    </row>
+    <row r="1010" spans="1:27">
+      <c r="A1010" s="6"/>
+      <c r="B1010" s="6"/>
+      <c r="C1010" s="6"/>
+      <c r="D1010" s="6"/>
+      <c r="E1010" s="6"/>
+      <c r="F1010" s="6"/>
+      <c r="G1010" s="6"/>
+      <c r="H1010" s="6"/>
+      <c r="I1010" s="6"/>
+      <c r="J1010" s="6"/>
+      <c r="K1010" s="6"/>
+      <c r="L1010" s="6"/>
+      <c r="M1010" s="6"/>
+      <c r="N1010" s="6"/>
+      <c r="O1010" s="6"/>
+      <c r="P1010" s="6"/>
+      <c r="Q1010" s="6"/>
+      <c r="R1010" s="6"/>
+      <c r="S1010" s="6"/>
+      <c r="T1010" s="6"/>
+      <c r="U1010" s="6"/>
+      <c r="V1010" s="6"/>
+      <c r="W1010" s="6"/>
+      <c r="X1010" s="6"/>
+      <c r="Y1010" s="6"/>
+      <c r="Z1010" s="6"/>
+      <c r="AA1010" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -32606,35 +33138,47 @@
     <hyperlink ref="B47" r:id="rId46"/>
     <hyperlink ref="B48" r:id="rId47"/>
     <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53" location="SanitationMethods"/>
-    <hyperlink ref="B55" r:id="rId54" location="SanitationMethods"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B64" r:id="rId63"/>
-    <hyperlink ref="B65" r:id="rId64"/>
-    <hyperlink ref="B66" r:id="rId65"/>
-    <hyperlink ref="B67" r:id="rId66"/>
-    <hyperlink ref="B68" r:id="rId67"/>
-    <hyperlink ref="B69" r:id="rId68"/>
-    <hyperlink ref="B70" r:id="rId69"/>
-    <hyperlink ref="B71" r:id="rId70"/>
-    <hyperlink ref="B72" r:id="rId71"/>
-    <hyperlink ref="B73" r:id="rId72"/>
-    <hyperlink ref="B74" r:id="rId73"/>
-    <hyperlink ref="B75" r:id="rId74"/>
-    <hyperlink ref="B76" r:id="rId75"/>
+    <hyperlink ref="B51" r:id="rId49"/>
+    <hyperlink ref="B52" r:id="rId50"/>
+    <hyperlink ref="B53" r:id="rId51"/>
+    <hyperlink ref="B54" r:id="rId52"/>
+    <hyperlink ref="B55" r:id="rId53" location="SanitationMethods"/>
+    <hyperlink ref="B56" r:id="rId54" location="SanitationMethods"/>
+    <hyperlink ref="B57" r:id="rId55"/>
+    <hyperlink ref="B58" r:id="rId56"/>
+    <hyperlink ref="B59" r:id="rId57"/>
+    <hyperlink ref="B60" r:id="rId58"/>
+    <hyperlink ref="B61" r:id="rId59"/>
+    <hyperlink ref="B62" r:id="rId60"/>
+    <hyperlink ref="B63" r:id="rId61"/>
+    <hyperlink ref="B64" r:id="rId62"/>
+    <hyperlink ref="B65" r:id="rId63"/>
+    <hyperlink ref="B66" r:id="rId64"/>
+    <hyperlink ref="B67" r:id="rId65"/>
+    <hyperlink ref="B68" r:id="rId66"/>
+    <hyperlink ref="B69" r:id="rId67"/>
+    <hyperlink ref="B70" r:id="rId68"/>
+    <hyperlink ref="B71" r:id="rId69"/>
+    <hyperlink ref="B72" r:id="rId70"/>
+    <hyperlink ref="B73" r:id="rId71"/>
+    <hyperlink ref="B75" r:id="rId72"/>
+    <hyperlink ref="B76" r:id="rId73"/>
+    <hyperlink ref="B77" r:id="rId74"/>
+    <hyperlink ref="B80" r:id="rId75"/>
+    <hyperlink ref="B50" r:id="rId76"/>
+    <hyperlink ref="B74" r:id="rId77"/>
+    <hyperlink ref="B78" r:id="rId78"/>
+    <hyperlink ref="B79" r:id="rId79" display="https://demoqa.com/menu"/>
+    <hyperlink ref="B81" r:id="rId80"/>
+    <hyperlink ref="B82" r:id="rId81"/>
+    <hyperlink ref="B83" r:id="rId82"/>
+    <hyperlink ref="B84" r:id="rId83"/>
+    <hyperlink ref="B85" r:id="rId84"/>
+    <hyperlink ref="B86" r:id="rId85"/>
+    <hyperlink ref="B87" r:id="rId86"/>
+    <hyperlink ref="B88" r:id="rId87"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId76"/>
+  <pageSetup orientation="portrait" r:id="rId88"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TestCases For JoyBird with updated code
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -1396,7 +1396,7 @@
     <t>span:contains(Showrooms)</t>
   </si>
   <si>
-    <t>(//span[contains(text(), 'Showrooms')])[1]</t>
+    <t>//span[contains(text(), 'Showrooms')]</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1759,9 @@
   </sheetPr>
   <dimension ref="A1:AA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1768,7 +1769,7 @@
     <col min="1" max="1" width="17.21875" customWidth="1"/>
     <col min="2" max="2" width="39.77734375" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" customWidth="1"/>
@@ -5780,7 +5781,7 @@
       <c r="Z79" s="6"/>
       <c r="AA79" s="6"/>
     </row>
-    <row r="80" spans="1:27" ht="119.4" thickBot="1">
+    <row r="80" spans="1:27" ht="93" thickBot="1">
       <c r="A80" s="12" t="s">
         <v>256</v>
       </c>

</xml_diff>

<commit_message>
these files are overridden
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -739,30 +739,12 @@
     <t>ABHI_VYAKTI_02</t>
   </si>
   <si>
-    <t>div[class*='col-lg-']:nth-of-type(1) div[class='box-border']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'col-lg-')][1]/div[@class='box-border']</t>
-  </si>
-  <si>
-    <t>div[class*='col-lg-'] div[class='box-border']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'col-lg-')]/div[@class='box-border']</t>
-  </si>
-  <si>
     <t>ABHI_VYAKTI_03</t>
   </si>
   <si>
-    <t>div[class*='col-md-']:nth-of-type(4)&gt;a:nth-of-type(1)</t>
-  </si>
-  <si>
     <t>//div[contains(@class, 'col-md-')][4]/a[1]</t>
   </si>
   <si>
-    <t>div[class*='col-md-']&gt;a</t>
-  </si>
-  <si>
     <t>//div[contains(@class, 'col-md-')]/a</t>
   </si>
   <si>
@@ -1535,6 +1517,24 @@
   </si>
   <si>
     <t>button[class*='group']:nth-of-type(5) &gt; span[class*='leading-']</t>
+  </si>
+  <si>
+    <t>div[class*='col-lg-']:nth-of-type(1) img[alt='garba mahotsav']</t>
+  </si>
+  <si>
+    <t>//div[contains(@class, 'col-lg-')][1]//img[@alt='garba mahotsav']</t>
+  </si>
+  <si>
+    <t>div[class*='col-lg-'] img[alt='garba mahotsav']</t>
+  </si>
+  <si>
+    <t>//div[contains(@class, 'col-lg-')]//img[@alt='garba mahotsav']</t>
+  </si>
+  <si>
+    <t>div[class*='col-md-']:nth-of-type(4) &gt; a:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>div[class*='col-md-'] &gt; a</t>
   </si>
 </sst>
 </file>
@@ -1902,8 +1902,8 @@
   <dimension ref="A1:AA1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1985,22 +1985,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>15</v>
@@ -2036,22 +2036,22 @@
         <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>15</v>
@@ -2093,10 +2093,10 @@
         <v>23</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>24</v>
@@ -2138,22 +2138,22 @@
         <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>15</v>
@@ -2189,16 +2189,16 @@
         <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>32</v>
@@ -2246,16 +2246,16 @@
         <v>39</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>40</v>
@@ -2297,16 +2297,16 @@
         <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>15</v>
@@ -2348,10 +2348,10 @@
         <v>50</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>51</v>
@@ -2399,10 +2399,10 @@
         <v>58</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>59</v>
@@ -2447,13 +2447,13 @@
         <v>64</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>65</v>
@@ -2495,22 +2495,22 @@
         <v>69</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>53</v>
@@ -2552,16 +2552,16 @@
         <v>74</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>53</v>
@@ -2603,10 +2603,10 @@
         <v>78</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>79</v>
@@ -2654,10 +2654,10 @@
         <v>85</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>86</v>
@@ -2705,10 +2705,10 @@
         <v>92</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>93</v>
@@ -2756,16 +2756,16 @@
         <v>99</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>88</v>
@@ -2801,22 +2801,22 @@
         <v>102</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>103</v>
@@ -2852,16 +2852,16 @@
         <v>106</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>107</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>108</v>
@@ -2900,7 +2900,7 @@
         <v>111</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>112</v>
@@ -2909,10 +2909,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>114</v>
@@ -2954,22 +2954,22 @@
         <v>117</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>118</v>
@@ -3005,22 +3005,22 @@
         <v>120</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>121</v>
@@ -3062,10 +3062,10 @@
         <v>126</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>127</v>
@@ -3101,7 +3101,7 @@
         <v>35</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>130</v>
@@ -3113,16 +3113,16 @@
         <v>132</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>121</v>
@@ -3152,22 +3152,22 @@
         <v>134</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>136</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>137</v>
@@ -3203,22 +3203,22 @@
         <v>134</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>140</v>
@@ -3254,7 +3254,7 @@
         <v>134</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>143</v>
@@ -3266,16 +3266,16 @@
         <v>145</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>121</v>
@@ -3305,7 +3305,7 @@
         <v>134</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>147</v>
@@ -3317,16 +3317,16 @@
         <v>149</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>121</v>
@@ -3356,28 +3356,28 @@
         <v>151</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>152</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>121</v>
@@ -3407,28 +3407,28 @@
         <v>155</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>121</v>
@@ -3458,22 +3458,22 @@
         <v>157</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>158</v>
@@ -3521,10 +3521,10 @@
         <v>165</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>166</v>
@@ -3566,16 +3566,16 @@
         <v>170</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>171</v>
@@ -3611,22 +3611,22 @@
         <v>161</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>176</v>
@@ -3674,10 +3674,10 @@
         <v>165</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>181</v>
@@ -3713,28 +3713,28 @@
         <v>184</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>121</v>
@@ -3770,16 +3770,16 @@
         <v>188</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>189</v>
@@ -3821,16 +3821,16 @@
         <v>193</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>194</v>
@@ -3878,10 +3878,10 @@
         <v>200</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>201</v>
@@ -3929,16 +3929,16 @@
         <v>208</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>121</v>
@@ -3968,22 +3968,22 @@
         <v>184</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>211</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>212</v>
@@ -4019,22 +4019,22 @@
         <v>184</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>216</v>
@@ -4076,22 +4076,22 @@
         <v>221</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>121</v>
@@ -4121,28 +4121,28 @@
         <v>223</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>121</v>
@@ -4178,22 +4178,22 @@
         <v>226</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>121</v>
@@ -4226,25 +4226,25 @@
         <v>226</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>121</v>
@@ -4280,22 +4280,22 @@
         <v>230</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>121</v>
@@ -4325,28 +4325,28 @@
         <v>225</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>232</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>121</v>
@@ -4376,24 +4376,24 @@
         <v>225</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I49" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="J49" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>504</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>121</v>
@@ -4417,30 +4417,30 @@
     </row>
     <row r="50" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A50" s="11" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50" s="11"/>
@@ -4478,16 +4478,16 @@
         <v>239</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K51" s="5" t="s">
         <v>121</v>
@@ -4509,7 +4509,7 @@
       <c r="Z51" s="5"/>
       <c r="AA51" s="5"/>
     </row>
-    <row r="52" spans="1:27" ht="52.8">
+    <row r="52" spans="1:27" ht="66">
       <c r="A52" s="3" t="s">
         <v>240</v>
       </c>
@@ -4517,28 +4517,28 @@
         <v>235</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>241</v>
+        <v>501</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>242</v>
+        <v>502</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>243</v>
+        <v>503</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>244</v>
+        <v>504</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>121</v>
@@ -4562,34 +4562,34 @@
     </row>
     <row r="53" spans="1:27" ht="39.6">
       <c r="A53" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>235</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>246</v>
+        <v>505</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>248</v>
+        <v>506</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="K53" s="5" t="s">
         <v>121</v>
@@ -4613,37 +4613,37 @@
     </row>
     <row r="54" spans="1:27" ht="264">
       <c r="A54" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>235</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
@@ -4664,37 +4664,37 @@
     </row>
     <row r="55" spans="1:27" ht="158.4">
       <c r="A55" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I55" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="J55" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="K55" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -4715,37 +4715,37 @@
     </row>
     <row r="56" spans="1:27" ht="158.4">
       <c r="A56" s="5" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
@@ -4766,34 +4766,34 @@
     </row>
     <row r="57" spans="1:27" ht="26.4">
       <c r="A57" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I57" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="J57" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>280</v>
       </c>
       <c r="K57" s="5" t="s">
         <v>121</v>
@@ -4817,34 +4817,34 @@
     </row>
     <row r="58" spans="1:27" ht="26.4">
       <c r="A58" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="J58" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>287</v>
       </c>
       <c r="K58" s="5" t="s">
         <v>121</v>
@@ -4868,37 +4868,37 @@
     </row>
     <row r="59" spans="1:27" ht="52.8">
       <c r="A59" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I59" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="J59" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>295</v>
-      </c>
       <c r="K59" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
@@ -4919,37 +4919,37 @@
     </row>
     <row r="60" spans="1:27" ht="26.4">
       <c r="A60" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -4970,34 +4970,34 @@
     </row>
     <row r="61" spans="1:27" ht="26.4">
       <c r="A61" s="5" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>121</v>
@@ -5021,37 +5021,37 @@
     </row>
     <row r="62" spans="1:27" ht="39.6">
       <c r="A62" s="5" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
@@ -5072,34 +5072,34 @@
     </row>
     <row r="63" spans="1:27" ht="52.8">
       <c r="A63" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="J63" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>314</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>121</v>
@@ -5123,34 +5123,34 @@
     </row>
     <row r="64" spans="1:27" ht="52.8">
       <c r="A64" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="J64" s="5" t="s">
         <v>315</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>321</v>
       </c>
       <c r="K64" s="5" t="s">
         <v>121</v>
@@ -5174,34 +5174,34 @@
     </row>
     <row r="65" spans="1:27" ht="52.8">
       <c r="A65" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="J65" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>328</v>
       </c>
       <c r="K65" s="5" t="s">
         <v>121</v>
@@ -5225,34 +5225,34 @@
     </row>
     <row r="66" spans="1:27" ht="13.2">
       <c r="A66" s="3" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>121</v>
@@ -5276,40 +5276,40 @@
     </row>
     <row r="67" spans="1:27" ht="92.4">
       <c r="A67" s="3" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B67" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>336</v>
-      </c>
       <c r="G67" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>121</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
@@ -5329,34 +5329,34 @@
     </row>
     <row r="68" spans="1:27" ht="79.2">
       <c r="A68" s="3" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K68" s="5" t="s">
         <v>121</v>
@@ -5380,34 +5380,34 @@
     </row>
     <row r="69" spans="1:27" ht="79.2">
       <c r="A69" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="J69" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>121</v>
@@ -5431,34 +5431,34 @@
     </row>
     <row r="70" spans="1:27" ht="13.2">
       <c r="A70" s="3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K70" s="5" t="s">
         <v>121</v>
@@ -5482,40 +5482,40 @@
     </row>
     <row r="71" spans="1:27" ht="66">
       <c r="A71" s="3" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>121</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
@@ -5535,34 +5535,34 @@
     </row>
     <row r="72" spans="1:27" ht="66">
       <c r="A72" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J72" s="5" t="s">
         <v>359</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>365</v>
       </c>
       <c r="K72" s="5" t="s">
         <v>121</v>
@@ -5586,34 +5586,34 @@
     </row>
     <row r="73" spans="1:27" ht="106.2" thickBot="1">
       <c r="A73" s="5" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="K73" s="5" t="s">
         <v>121</v>
@@ -5637,22 +5637,22 @@
     </row>
     <row r="74" spans="1:27" ht="106.2" thickBot="1">
       <c r="A74" s="11" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
@@ -5662,7 +5662,7 @@
         <v>121</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
@@ -5682,34 +5682,34 @@
     </row>
     <row r="75" spans="1:27" ht="118.8">
       <c r="A75" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I75" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="J75" s="5" t="s">
         <v>373</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>379</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>121</v>
@@ -5733,34 +5733,34 @@
     </row>
     <row r="76" spans="1:27" ht="39.6">
       <c r="A76" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I76" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="J76" s="5" t="s">
         <v>381</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H76" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>387</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>121</v>
@@ -5784,34 +5784,34 @@
     </row>
     <row r="77" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A77" s="5" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="K77" s="5" t="s">
         <v>121</v>
@@ -5835,36 +5835,36 @@
     </row>
     <row r="78" spans="1:27" ht="145.80000000000001" thickBot="1">
       <c r="A78" s="11" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M78" s="11"/>
       <c r="N78" s="11"/>
@@ -5884,36 +5884,36 @@
     </row>
     <row r="79" spans="1:27" ht="27" thickBot="1">
       <c r="A79" s="11" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="J79" s="11" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="K79" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
@@ -5933,34 +5933,34 @@
     </row>
     <row r="80" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A80" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I80" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="J80" s="5" t="s">
         <v>394</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>400</v>
       </c>
       <c r="K80" s="5" t="s">
         <v>121</v>
@@ -5984,34 +5984,34 @@
     </row>
     <row r="81" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A81" s="11" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="13" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="K81" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L81" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M81" s="11"/>
       <c r="N81" s="11"/>
@@ -6031,22 +6031,22 @@
     </row>
     <row r="82" spans="1:27" ht="79.8" thickBot="1">
       <c r="A82" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
@@ -6056,7 +6056,7 @@
         <v>121</v>
       </c>
       <c r="L82" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M82" s="11"/>
       <c r="N82" s="11"/>
@@ -6076,16 +6076,16 @@
     </row>
     <row r="83" spans="1:27" ht="27" thickBot="1">
       <c r="A83" s="11" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -6094,10 +6094,10 @@
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L83" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M83" s="11"/>
       <c r="N83" s="11"/>
@@ -6117,36 +6117,36 @@
     </row>
     <row r="84" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A84" s="11" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="B84" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="E84" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="C84" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>459</v>
-      </c>
       <c r="F84" s="11" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="J84" s="11" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L84" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M84" s="11"/>
       <c r="N84" s="11"/>
@@ -6166,22 +6166,22 @@
     </row>
     <row r="85" spans="1:27" ht="79.8" thickBot="1">
       <c r="A85" s="11" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -6189,7 +6189,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="11"/>
       <c r="L85" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M85" s="11"/>
       <c r="N85" s="11"/>
@@ -6209,16 +6209,16 @@
     </row>
     <row r="86" spans="1:27" ht="93" thickBot="1">
       <c r="A86" s="11" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B86" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="C86" s="11" t="s">
-        <v>470</v>
-      </c>
       <c r="D86" s="11" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -6228,7 +6228,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="11"/>
       <c r="L86" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M86" s="11"/>
       <c r="N86" s="11"/>
@@ -6248,34 +6248,34 @@
     </row>
     <row r="87" spans="1:27" ht="277.8" thickBot="1">
       <c r="A87" s="11" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="K87" s="11"/>
       <c r="L87" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M87" s="11"/>
       <c r="N87" s="11"/>
@@ -6295,16 +6295,16 @@
     </row>
     <row r="88" spans="1:27" ht="27" thickBot="1">
       <c r="A88" s="11" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
@@ -6314,7 +6314,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="11"/>
       <c r="L88" s="11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="M88" s="11"/>
       <c r="N88" s="11"/>

</xml_diff>

<commit_message>
EPFO test case coomit
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -844,15 +844,9 @@
     <t>EPFO_02</t>
   </si>
   <si>
-    <t>div[id='footer_link'] a:nth-of-type(1)</t>
-  </si>
-  <si>
     <t>//div[@id='footer_link']/a[1]</t>
   </si>
   <si>
-    <t>div[id='footer_link'] a</t>
-  </si>
-  <si>
     <t>//div[@id='footer_link']/a</t>
   </si>
   <si>
@@ -868,15 +862,9 @@
     <t>https://www.epfindia.gov.in/site_en/International_workers.php</t>
   </si>
   <si>
-    <t>div[class='iternl_wrkr'] span[class='nor_letter']:nth-of-type(2)</t>
-  </si>
-  <si>
     <t>//div[@class='iternl_wrkr']/span[@class='nor_letter'][1]</t>
   </si>
   <si>
-    <t>div[class='iternl_wrkr'] span[class='nor_letter']</t>
-  </si>
-  <si>
     <t>//div[@class='iternl_wrkr']/span[@class='nor_letter']</t>
   </si>
   <si>
@@ -1535,6 +1523,18 @@
   </si>
   <si>
     <t>div[class*='col-md-'] &gt; a</t>
+  </si>
+  <si>
+    <t>div[id='footer_link'] &gt; a:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>div[id='footer_link'] &gt; a</t>
+  </si>
+  <si>
+    <t>div[class='iternl_wrkr'] &gt; span[class='nor_letter']:nth-of-type(2)</t>
+  </si>
+  <si>
+    <t>div[class='iternl_wrkr'] &gt; span[class='nor_letter']</t>
   </si>
 </sst>
 </file>
@@ -1901,9 +1901,9 @@
   </sheetPr>
   <dimension ref="A1:AA1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1985,22 +1985,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>15</v>
@@ -2036,22 +2036,22 @@
         <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>15</v>
@@ -2093,10 +2093,10 @@
         <v>23</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>24</v>
@@ -2138,22 +2138,22 @@
         <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>15</v>
@@ -2189,16 +2189,16 @@
         <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>32</v>
@@ -2246,16 +2246,16 @@
         <v>39</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>40</v>
@@ -2297,16 +2297,16 @@
         <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>15</v>
@@ -2348,10 +2348,10 @@
         <v>50</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>51</v>
@@ -2399,10 +2399,10 @@
         <v>58</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>59</v>
@@ -2447,13 +2447,13 @@
         <v>64</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>65</v>
@@ -2495,22 +2495,22 @@
         <v>69</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>53</v>
@@ -2552,16 +2552,16 @@
         <v>74</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>53</v>
@@ -2603,10 +2603,10 @@
         <v>78</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>79</v>
@@ -2654,10 +2654,10 @@
         <v>85</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>86</v>
@@ -2705,10 +2705,10 @@
         <v>92</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>93</v>
@@ -2756,16 +2756,16 @@
         <v>99</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>88</v>
@@ -2801,22 +2801,22 @@
         <v>102</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>103</v>
@@ -2852,16 +2852,16 @@
         <v>106</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>107</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>108</v>
@@ -2900,7 +2900,7 @@
         <v>111</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>112</v>
@@ -2909,10 +2909,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>114</v>
@@ -2954,22 +2954,22 @@
         <v>117</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>118</v>
@@ -3005,22 +3005,22 @@
         <v>120</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>121</v>
@@ -3062,10 +3062,10 @@
         <v>126</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>127</v>
@@ -3101,7 +3101,7 @@
         <v>35</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>130</v>
@@ -3113,16 +3113,16 @@
         <v>132</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>121</v>
@@ -3152,22 +3152,22 @@
         <v>134</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>136</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>137</v>
@@ -3203,22 +3203,22 @@
         <v>134</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>140</v>
@@ -3254,7 +3254,7 @@
         <v>134</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>143</v>
@@ -3266,16 +3266,16 @@
         <v>145</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>121</v>
@@ -3305,7 +3305,7 @@
         <v>134</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>147</v>
@@ -3317,16 +3317,16 @@
         <v>149</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>121</v>
@@ -3356,28 +3356,28 @@
         <v>151</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>152</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>121</v>
@@ -3407,28 +3407,28 @@
         <v>155</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>121</v>
@@ -3458,22 +3458,22 @@
         <v>157</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>158</v>
@@ -3521,10 +3521,10 @@
         <v>165</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>166</v>
@@ -3566,16 +3566,16 @@
         <v>170</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>171</v>
@@ -3611,22 +3611,22 @@
         <v>161</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>176</v>
@@ -3674,10 +3674,10 @@
         <v>165</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>181</v>
@@ -3713,28 +3713,28 @@
         <v>184</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>121</v>
@@ -3770,16 +3770,16 @@
         <v>188</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>189</v>
@@ -3821,16 +3821,16 @@
         <v>193</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>194</v>
@@ -3878,10 +3878,10 @@
         <v>200</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>201</v>
@@ -3929,16 +3929,16 @@
         <v>208</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>121</v>
@@ -3968,22 +3968,22 @@
         <v>184</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>211</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>212</v>
@@ -4019,22 +4019,22 @@
         <v>184</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>216</v>
@@ -4076,22 +4076,22 @@
         <v>221</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>121</v>
@@ -4121,28 +4121,28 @@
         <v>223</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>121</v>
@@ -4178,22 +4178,22 @@
         <v>226</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>121</v>
@@ -4226,25 +4226,25 @@
         <v>226</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>121</v>
@@ -4280,22 +4280,22 @@
         <v>230</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>121</v>
@@ -4325,28 +4325,28 @@
         <v>225</v>
       </c>
       <c r="C48" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>497</v>
-      </c>
       <c r="E48" s="5" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>232</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>121</v>
@@ -4376,24 +4376,24 @@
         <v>225</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>121</v>
@@ -4417,30 +4417,30 @@
     </row>
     <row r="50" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A50" s="11" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50" s="11"/>
@@ -4478,16 +4478,16 @@
         <v>239</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K51" s="5" t="s">
         <v>121</v>
@@ -4517,28 +4517,28 @@
         <v>235</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>121</v>
@@ -4568,22 +4568,22 @@
         <v>235</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>242</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>243</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>244</v>
@@ -4631,10 +4631,10 @@
         <v>250</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>251</v>
@@ -4643,7 +4643,7 @@
         <v>252</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
@@ -4682,10 +4682,10 @@
         <v>258</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>259</v>
@@ -4727,16 +4727,16 @@
         <v>264</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>265</v>
@@ -4784,10 +4784,10 @@
         <v>272</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>273</v>
@@ -4823,28 +4823,28 @@
         <v>268</v>
       </c>
       <c r="C58" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="E58" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="G58" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I58" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="J58" s="5" t="s">
         <v>279</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="K58" s="5" t="s">
         <v>121</v>
@@ -4868,34 +4868,34 @@
     </row>
     <row r="59" spans="1:27" ht="52.8">
       <c r="A59" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="E59" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="G59" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I59" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="J59" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>289</v>
       </c>
       <c r="K59" s="5" t="s">
         <v>261</v>
@@ -4919,34 +4919,34 @@
     </row>
     <row r="60" spans="1:27" ht="26.4">
       <c r="A60" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K60" s="5" t="s">
         <v>261</v>
@@ -4970,34 +4970,34 @@
     </row>
     <row r="61" spans="1:27" ht="26.4">
       <c r="A61" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>121</v>
@@ -5021,34 +5021,34 @@
     </row>
     <row r="62" spans="1:27" ht="39.6">
       <c r="A62" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="G62" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K62" s="5" t="s">
         <v>261</v>
@@ -5072,34 +5072,34 @@
     </row>
     <row r="63" spans="1:27" ht="52.8">
       <c r="A63" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C63" s="5" t="s">
+      <c r="G63" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I63" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="J63" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>121</v>
@@ -5123,34 +5123,34 @@
     </row>
     <row r="64" spans="1:27" ht="52.8">
       <c r="A64" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C64" s="5" t="s">
+      <c r="G64" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I64" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="J64" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>315</v>
       </c>
       <c r="K64" s="5" t="s">
         <v>121</v>
@@ -5174,34 +5174,34 @@
     </row>
     <row r="65" spans="1:27" ht="52.8">
       <c r="A65" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C65" s="5" t="s">
+      <c r="G65" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I65" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="J65" s="5" t="s">
         <v>318</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>322</v>
       </c>
       <c r="K65" s="5" t="s">
         <v>121</v>
@@ -5225,34 +5225,34 @@
     </row>
     <row r="66" spans="1:27" ht="13.2">
       <c r="A66" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>121</v>
@@ -5276,40 +5276,40 @@
     </row>
     <row r="67" spans="1:27" ht="92.4">
       <c r="A67" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>330</v>
-      </c>
       <c r="G67" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>121</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
@@ -5329,34 +5329,34 @@
     </row>
     <row r="68" spans="1:27" ht="79.2">
       <c r="A68" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>336</v>
-      </c>
       <c r="G68" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K68" s="5" t="s">
         <v>121</v>
@@ -5380,34 +5380,34 @@
     </row>
     <row r="69" spans="1:27" ht="79.2">
       <c r="A69" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C69" s="5" t="s">
+      <c r="G69" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I69" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="J69" s="5" t="s">
         <v>339</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>343</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>121</v>
@@ -5431,34 +5431,34 @@
     </row>
     <row r="70" spans="1:27" ht="13.2">
       <c r="A70" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K70" s="5" t="s">
         <v>121</v>
@@ -5482,40 +5482,40 @@
     </row>
     <row r="71" spans="1:27" ht="66">
       <c r="A71" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F71" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>351</v>
-      </c>
       <c r="G71" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>121</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
@@ -5535,34 +5535,34 @@
     </row>
     <row r="72" spans="1:27" ht="66">
       <c r="A72" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="F72" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C72" s="5" t="s">
+      <c r="G72" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I72" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="J72" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>359</v>
       </c>
       <c r="K72" s="5" t="s">
         <v>121</v>
@@ -5586,34 +5586,34 @@
     </row>
     <row r="73" spans="1:27" ht="106.2" thickBot="1">
       <c r="A73" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="K73" s="5" t="s">
         <v>121</v>
@@ -5637,22 +5637,22 @@
     </row>
     <row r="74" spans="1:27" ht="106.2" thickBot="1">
       <c r="A74" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="F74" s="11" t="s">
         <v>413</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>417</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
@@ -5662,7 +5662,7 @@
         <v>121</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
@@ -5682,34 +5682,34 @@
     </row>
     <row r="75" spans="1:27" ht="118.8">
       <c r="A75" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="F75" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="G75" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I75" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="J75" s="5" t="s">
         <v>369</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>373</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>121</v>
@@ -5733,34 +5733,34 @@
     </row>
     <row r="76" spans="1:27" ht="39.6">
       <c r="A76" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="F76" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="G76" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I76" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="J76" s="5" t="s">
         <v>377</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H76" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>381</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>121</v>
@@ -5784,34 +5784,34 @@
     </row>
     <row r="77" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A77" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="J77" s="5" t="s">
         <v>382</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>386</v>
       </c>
       <c r="K77" s="5" t="s">
         <v>121</v>
@@ -5835,36 +5835,36 @@
     </row>
     <row r="78" spans="1:27" ht="145.80000000000001" thickBot="1">
       <c r="A78" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="E78" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="F78" s="11" t="s">
         <v>420</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>424</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M78" s="11"/>
       <c r="N78" s="11"/>
@@ -5884,36 +5884,36 @@
     </row>
     <row r="79" spans="1:27" ht="27" thickBot="1">
       <c r="A79" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="E79" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="F79" s="11" t="s">
         <v>428</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="E79" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="F79" s="11" t="s">
-        <v>432</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J79" s="11" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K79" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
@@ -5933,34 +5933,34 @@
     </row>
     <row r="80" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A80" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="F80" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="G80" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I80" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="J80" s="5" t="s">
         <v>390</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>394</v>
       </c>
       <c r="K80" s="5" t="s">
         <v>121</v>
@@ -5984,34 +5984,34 @@
     </row>
     <row r="81" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A81" s="11" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="13" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="K81" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L81" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M81" s="11"/>
       <c r="N81" s="11"/>
@@ -6031,22 +6031,22 @@
     </row>
     <row r="82" spans="1:27" ht="79.8" thickBot="1">
       <c r="A82" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="F82" s="11" t="s">
         <v>441</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="F82" s="11" t="s">
-        <v>445</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
@@ -6056,7 +6056,7 @@
         <v>121</v>
       </c>
       <c r="L82" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M82" s="11"/>
       <c r="N82" s="11"/>
@@ -6076,16 +6076,16 @@
     </row>
     <row r="83" spans="1:27" ht="27" thickBot="1">
       <c r="A83" s="11" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -6097,7 +6097,7 @@
         <v>261</v>
       </c>
       <c r="L83" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M83" s="11"/>
       <c r="N83" s="11"/>
@@ -6117,36 +6117,36 @@
     </row>
     <row r="84" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A84" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="F84" s="11" t="s">
         <v>450</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>454</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J84" s="11" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L84" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M84" s="11"/>
       <c r="N84" s="11"/>
@@ -6166,22 +6166,22 @@
     </row>
     <row r="85" spans="1:27" ht="79.8" thickBot="1">
       <c r="A85" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="E85" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="F85" s="11" t="s">
         <v>458</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>462</v>
       </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -6189,7 +6189,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="11"/>
       <c r="L85" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M85" s="11"/>
       <c r="N85" s="11"/>
@@ -6209,16 +6209,16 @@
     </row>
     <row r="86" spans="1:27" ht="93" thickBot="1">
       <c r="A86" s="11" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -6228,7 +6228,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="11"/>
       <c r="L86" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M86" s="11"/>
       <c r="N86" s="11"/>
@@ -6248,34 +6248,34 @@
     </row>
     <row r="87" spans="1:27" ht="277.8" thickBot="1">
       <c r="A87" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="F87" s="11" t="s">
         <v>466</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>458</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>468</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>470</v>
       </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="K87" s="11"/>
       <c r="L87" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M87" s="11"/>
       <c r="N87" s="11"/>
@@ -6295,16 +6295,16 @@
     </row>
     <row r="88" spans="1:27" ht="27" thickBot="1">
       <c r="A88" s="11" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
@@ -6314,7 +6314,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="11"/>
       <c r="L88" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M88" s="11"/>
       <c r="N88" s="11"/>

</xml_diff>

<commit_message>
added files of rgpv
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -742,15 +742,9 @@
     <t>ABHI_VYAKTI_03</t>
   </si>
   <si>
-    <t>div[class*='col-md-']:nth-of-type(4)&gt;a:nth-of-type(1)</t>
-  </si>
-  <si>
     <t>//div[contains(@class, 'col-md-')][4]/a[1]</t>
   </si>
   <si>
-    <t>div[class*='col-md-']&gt;a</t>
-  </si>
-  <si>
     <t>//div[contains(@class, 'col-md-')]/a</t>
   </si>
   <si>
@@ -907,27 +901,12 @@
     <t>https://jeevanpramaan.gov.in/</t>
   </si>
   <si>
-    <t>li[class='year'] i[class='fa fa-pencil']</t>
-  </si>
-  <si>
-    <t>//li[@class='year'][1]/i[@class='fa fa-pencil']</t>
-  </si>
-  <si>
-    <t>//li[@class='year']/i[@class='fa fa-pencil']</t>
-  </si>
-  <si>
     <t>JEEVAN_PRAMAAN_03</t>
   </si>
   <si>
-    <t>ul[class='nav main-nav'] li:nth-of-type(4) a[class='scroll']</t>
-  </si>
-  <si>
     <t>//ul[@class='nav main-nav']/li[4]/a[@class='scroll']</t>
   </si>
   <si>
-    <t>ul[class='nav main-nav'] li a[class='scroll']</t>
-  </si>
-  <si>
     <t>//ul[@class='nav main-nav']/li/a[@class='scroll']</t>
   </si>
   <si>
@@ -1538,6 +1517,27 @@
   </si>
   <si>
     <t>div[class='iternl_wrkr'] &gt; span[class='nor_letter']</t>
+  </si>
+  <si>
+    <t>//li[@class='']/a[@class='scroll']</t>
+  </si>
+  <si>
+    <t>ul[class='nav main-nav']&gt;li&gt;a[class='scroll']</t>
+  </si>
+  <si>
+    <t>(//a[contains(text(), 'Home')])[1]</t>
+  </si>
+  <si>
+    <t>li[class] &gt; a[class='scroll']</t>
+  </si>
+  <si>
+    <t>ul[class='nav main-nav']&gt;li:nth-of-type(4)&gt;a[class='scroll']</t>
+  </si>
+  <si>
+    <t>div[class*='col-md-']:nth-of-type(4) &gt; a:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>div[class*='col-md-'] &gt; a</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1647,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1686,6 +1686,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1905,8 +1908,8 @@
   <dimension ref="A1:AA1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1988,22 +1991,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>15</v>
@@ -2039,22 +2042,22 @@
         <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>15</v>
@@ -2096,10 +2099,10 @@
         <v>23</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>24</v>
@@ -2141,22 +2144,22 @@
         <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>15</v>
@@ -2192,16 +2195,16 @@
         <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>32</v>
@@ -2249,16 +2252,16 @@
         <v>39</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>40</v>
@@ -2300,16 +2303,16 @@
         <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>15</v>
@@ -2351,10 +2354,10 @@
         <v>50</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>51</v>
@@ -2402,10 +2405,10 @@
         <v>58</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>59</v>
@@ -2450,13 +2453,13 @@
         <v>64</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>65</v>
@@ -2498,22 +2501,22 @@
         <v>69</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>53</v>
@@ -2555,16 +2558,16 @@
         <v>74</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>53</v>
@@ -2606,10 +2609,10 @@
         <v>78</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>79</v>
@@ -2657,10 +2660,10 @@
         <v>85</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>86</v>
@@ -2708,10 +2711,10 @@
         <v>92</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>93</v>
@@ -2759,16 +2762,16 @@
         <v>99</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>88</v>
@@ -2804,22 +2807,22 @@
         <v>102</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>103</v>
@@ -2855,16 +2858,16 @@
         <v>106</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>107</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>108</v>
@@ -2903,7 +2906,7 @@
         <v>111</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>112</v>
@@ -2912,10 +2915,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>114</v>
@@ -2957,22 +2960,22 @@
         <v>117</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>118</v>
@@ -3005,25 +3008,25 @@
         <v>120</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>121</v>
@@ -3053,22 +3056,22 @@
         <v>35</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>123</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>124</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>125</v>
@@ -3104,28 +3107,28 @@
         <v>35</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>128</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>129</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>121</v>
@@ -3155,22 +3158,22 @@
         <v>131</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>132</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>133</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>134</v>
@@ -3206,22 +3209,22 @@
         <v>131</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>137</v>
@@ -3257,22 +3260,22 @@
         <v>131</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>140</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>141</v>
@@ -3308,28 +3311,28 @@
         <v>131</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>144</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>145</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>121</v>
@@ -3359,28 +3362,28 @@
         <v>147</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>148</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>149</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>121</v>
@@ -3410,28 +3413,28 @@
         <v>151</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>121</v>
@@ -3461,22 +3464,22 @@
         <v>153</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>154</v>
@@ -3524,10 +3527,10 @@
         <v>161</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>162</v>
@@ -3569,16 +3572,16 @@
         <v>166</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>167</v>
@@ -3614,22 +3617,22 @@
         <v>157</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>170</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>171</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>172</v>
@@ -3677,10 +3680,10 @@
         <v>161</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>177</v>
@@ -3716,28 +3719,28 @@
         <v>180</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>181</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>121</v>
@@ -3773,16 +3776,16 @@
         <v>184</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>185</v>
@@ -3824,16 +3827,16 @@
         <v>189</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>190</v>
@@ -3881,10 +3884,10 @@
         <v>196</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>197</v>
@@ -3932,16 +3935,16 @@
         <v>204</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>121</v>
@@ -3971,22 +3974,22 @@
         <v>180</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>206</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>207</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>208</v>
@@ -4022,22 +4025,22 @@
         <v>180</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>212</v>
@@ -4079,22 +4082,22 @@
         <v>217</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>121</v>
@@ -4124,28 +4127,28 @@
         <v>219</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>121</v>
@@ -4181,22 +4184,22 @@
         <v>222</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>121</v>
@@ -4229,25 +4232,25 @@
         <v>222</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>121</v>
@@ -4283,22 +4286,22 @@
         <v>226</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>121</v>
@@ -4328,28 +4331,28 @@
         <v>221</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>228</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>121</v>
@@ -4379,24 +4382,24 @@
         <v>221</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>121</v>
@@ -4420,30 +4423,30 @@
     </row>
     <row r="50" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A50" s="11" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50" s="11"/>
@@ -4481,16 +4484,16 @@
         <v>235</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K51" s="5" t="s">
         <v>121</v>
@@ -4516,7 +4519,7 @@
       <c r="A52" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="14" t="s">
         <v>231</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -4532,16 +4535,16 @@
         <v>240</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>121</v>
@@ -4567,32 +4570,32 @@
       <c r="A53" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="14" t="s">
         <v>231</v>
       </c>
       <c r="C53" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="G53" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I53" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="J53" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>247</v>
       </c>
       <c r="K53" s="5" t="s">
         <v>121</v>
@@ -4616,37 +4619,37 @@
     </row>
     <row r="54" spans="1:27" ht="264">
       <c r="A54" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C54" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="F54" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="G54" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I54" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="J54" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>254</v>
-      </c>
       <c r="K54" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
@@ -4667,37 +4670,37 @@
     </row>
     <row r="55" spans="1:27" ht="158.4">
       <c r="A55" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="D55" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="F55" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="G55" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I55" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="J55" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="G55" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I55" s="5" t="s">
+      <c r="K55" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>263</v>
       </c>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -4718,37 +4721,37 @@
     </row>
     <row r="56" spans="1:27" ht="158.4">
       <c r="A56" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C56" s="5" t="s">
+      <c r="E56" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I56" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="J56" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="E56" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>268</v>
-      </c>
       <c r="K56" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
@@ -4769,34 +4772,34 @@
     </row>
     <row r="57" spans="1:27" ht="26.4">
       <c r="A57" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="D57" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="F57" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="G57" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I57" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="J57" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>276</v>
       </c>
       <c r="K57" s="5" t="s">
         <v>121</v>
@@ -4820,34 +4823,34 @@
     </row>
     <row r="58" spans="1:27" ht="26.4">
       <c r="A58" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="D58" s="5" t="s">
+      <c r="G58" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I58" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="E58" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="F58" s="5" t="s">
+      <c r="J58" s="5" t="s">
         <v>279</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="K58" s="5" t="s">
         <v>121</v>
@@ -4871,37 +4874,37 @@
     </row>
     <row r="59" spans="1:27" ht="52.8">
       <c r="A59" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="E59" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="D59" s="5" t="s">
+      <c r="G59" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I59" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="E59" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="F59" s="5" t="s">
+      <c r="J59" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="G59" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>287</v>
-      </c>
       <c r="K59" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
@@ -4922,37 +4925,37 @@
     </row>
     <row r="60" spans="1:27" ht="26.4">
       <c r="A60" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>290</v>
-      </c>
       <c r="E60" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -4973,34 +4976,34 @@
     </row>
     <row r="61" spans="1:27" ht="26.4">
       <c r="A61" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="D61" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>294</v>
-      </c>
       <c r="E61" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>121</v>
@@ -5024,37 +5027,37 @@
     </row>
     <row r="62" spans="1:27" ht="39.6">
       <c r="A62" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>297</v>
+        <v>504</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>298</v>
+        <v>501</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>393</v>
+        <v>502</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>299</v>
+        <v>58</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>393</v>
+        <v>278</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>393</v>
+        <v>503</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
@@ -5075,34 +5078,34 @@
     </row>
     <row r="63" spans="1:27" ht="52.8">
       <c r="A63" s="5" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="E63" s="5" t="s">
-        <v>303</v>
+        <v>502</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>121</v>
@@ -5126,34 +5129,34 @@
     </row>
     <row r="64" spans="1:27" ht="52.8">
       <c r="A64" s="5" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="K64" s="5" t="s">
         <v>121</v>
@@ -5177,34 +5180,34 @@
     </row>
     <row r="65" spans="1:27" ht="52.8">
       <c r="A65" s="5" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="K65" s="5" t="s">
         <v>121</v>
@@ -5228,34 +5231,34 @@
     </row>
     <row r="66" spans="1:27" ht="13.2">
       <c r="A66" s="3" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>121</v>
@@ -5279,40 +5282,40 @@
     </row>
     <row r="67" spans="1:27" ht="92.4">
       <c r="A67" s="3" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>121</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
@@ -5332,34 +5335,34 @@
     </row>
     <row r="68" spans="1:27" ht="79.2">
       <c r="A68" s="3" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K68" s="5" t="s">
         <v>121</v>
@@ -5383,34 +5386,34 @@
     </row>
     <row r="69" spans="1:27" ht="79.2">
       <c r="A69" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>121</v>
@@ -5434,34 +5437,34 @@
     </row>
     <row r="70" spans="1:27" ht="13.2">
       <c r="A70" s="3" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K70" s="5" t="s">
         <v>121</v>
@@ -5485,40 +5488,40 @@
     </row>
     <row r="71" spans="1:27" ht="66">
       <c r="A71" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>121</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
@@ -5538,34 +5541,34 @@
     </row>
     <row r="72" spans="1:27" ht="66">
       <c r="A72" s="5" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="K72" s="5" t="s">
         <v>121</v>
@@ -5589,34 +5592,34 @@
     </row>
     <row r="73" spans="1:27" ht="106.2" thickBot="1">
       <c r="A73" s="5" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="K73" s="5" t="s">
         <v>121</v>
@@ -5640,22 +5643,22 @@
     </row>
     <row r="74" spans="1:27" ht="106.2" thickBot="1">
       <c r="A74" s="11" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
@@ -5665,7 +5668,7 @@
         <v>121</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
@@ -5685,34 +5688,34 @@
     </row>
     <row r="75" spans="1:27" ht="118.8">
       <c r="A75" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="J75" s="5" t="s">
         <v>364</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>371</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>121</v>
@@ -5736,34 +5739,34 @@
     </row>
     <row r="76" spans="1:27" ht="39.6">
       <c r="A76" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="J76" s="5" t="s">
         <v>372</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H76" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>379</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>121</v>
@@ -5787,34 +5790,34 @@
     </row>
     <row r="77" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A77" s="5" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="K77" s="5" t="s">
         <v>121</v>
@@ -5838,36 +5841,36 @@
     </row>
     <row r="78" spans="1:27" ht="145.80000000000001" thickBot="1">
       <c r="A78" s="11" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M78" s="11"/>
       <c r="N78" s="11"/>
@@ -5887,36 +5890,36 @@
     </row>
     <row r="79" spans="1:27" ht="27" thickBot="1">
       <c r="A79" s="11" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="J79" s="11" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="K79" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
@@ -5936,34 +5939,34 @@
     </row>
     <row r="80" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A80" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="J80" s="5" t="s">
         <v>385</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>392</v>
       </c>
       <c r="K80" s="5" t="s">
         <v>121</v>
@@ -5987,34 +5990,34 @@
     </row>
     <row r="81" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A81" s="11" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="13" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="K81" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L81" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M81" s="11"/>
       <c r="N81" s="11"/>
@@ -6034,22 +6037,22 @@
     </row>
     <row r="82" spans="1:27" ht="79.8" thickBot="1">
       <c r="A82" s="11" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
@@ -6059,7 +6062,7 @@
         <v>121</v>
       </c>
       <c r="L82" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M82" s="11"/>
       <c r="N82" s="11"/>
@@ -6079,16 +6082,16 @@
     </row>
     <row r="83" spans="1:27" ht="27" thickBot="1">
       <c r="A83" s="11" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -6097,10 +6100,10 @@
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L83" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M83" s="11"/>
       <c r="N83" s="11"/>
@@ -6120,36 +6123,36 @@
     </row>
     <row r="84" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A84" s="11" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B84" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="F84" s="11" t="s">
         <v>445</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>450</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>452</v>
       </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="J84" s="11" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>121</v>
       </c>
       <c r="L84" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M84" s="11"/>
       <c r="N84" s="11"/>
@@ -6169,22 +6172,22 @@
     </row>
     <row r="85" spans="1:27" ht="79.8" thickBot="1">
       <c r="A85" s="11" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -6192,7 +6195,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="11"/>
       <c r="L85" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M85" s="11"/>
       <c r="N85" s="11"/>
@@ -6212,16 +6215,16 @@
     </row>
     <row r="86" spans="1:27" ht="93" thickBot="1">
       <c r="A86" s="11" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="B86" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="D86" s="11" t="s">
         <v>456</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>463</v>
       </c>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -6231,7 +6234,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="11"/>
       <c r="L86" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M86" s="11"/>
       <c r="N86" s="11"/>
@@ -6251,34 +6254,34 @@
     </row>
     <row r="87" spans="1:27" ht="277.8" thickBot="1">
       <c r="A87" s="11" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="K87" s="11"/>
       <c r="L87" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M87" s="11"/>
       <c r="N87" s="11"/>
@@ -6298,16 +6301,16 @@
     </row>
     <row r="88" spans="1:27" ht="27" thickBot="1">
       <c r="A88" s="11" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
@@ -6317,7 +6320,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="11"/>
       <c r="L88" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M88" s="11"/>
       <c r="N88" s="11"/>

</xml_diff>

<commit_message>
added rgpv test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="469">
   <si>
     <t>ID</t>
   </si>
@@ -949,36 +949,9 @@
     <t>UITRGPV_AC_02</t>
   </si>
   <si>
-    <t>div[class*='owl-item']:nth-of-type(13) div[class='courses_div'] img[class='img-fluid']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'owl-item')][13]//div[@class='courses_div']//img[@class='img-fluid']</t>
-  </si>
-  <si>
-    <t>div[class*='owl-item'] div[class='courses_div'] img[class='img-fluid']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'owl-item')]//div[@class='courses_div']//img[@class='img-fluid']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">civil engineering </t>
-  </si>
-  <si>
     <t>UITRGPV_AC_03</t>
   </si>
   <si>
-    <t>div[class*='owl-item']:nth-of-type(2) img[class*='w-']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'owl-item cloned')][2]//img[contains(@class, 'w-')]</t>
-  </si>
-  <si>
-    <t>div[class*='owl-item'] img[class*='w-']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'owl-item cloned')]//img[contains(@class, 'w-')]</t>
-  </si>
-  <si>
     <t>UITRGPV_AC_04</t>
   </si>
   <si>
@@ -1009,36 +982,9 @@
     <t>//a[@class='overlay-link play-now ripple']</t>
   </si>
   <si>
-    <t>UITRGPV_AC_06</t>
-  </si>
-  <si>
-    <t>div[class*='owl-item']:nth-of-type(10) div[class='facility_box']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'owl-item')][10]//div[@class='facility_box']</t>
-  </si>
-  <si>
-    <t>div[class*='owl-item'] div[class='facility_box']</t>
-  </si>
-  <si>
-    <t>//div[contains(@class, 'owl-item')]//div[@class='facility_box']</t>
-  </si>
-  <si>
-    <t>class room</t>
-  </si>
-  <si>
-    <t>UITRGPV_AC_07</t>
-  </si>
-  <si>
-    <t>div[class*='col-lg-']:nth-of-type(2) ul[class='list-item'] li:nth-of-type(1) a</t>
-  </si>
-  <si>
     <t>//div[contains(@class, 'col-lg-')][2]//ul[@class='list-item']/li[1]/a</t>
   </si>
   <si>
-    <t>div[class*='col-lg-'] ul[class='list-item'] li a</t>
-  </si>
-  <si>
     <t>//div[contains(@class, 'col-lg-')]//ul[@class='list-item']/li/a</t>
   </si>
   <si>
@@ -1048,24 +994,6 @@
     <t>//a[contains(text(), 'Photo Gallery')]</t>
   </si>
   <si>
-    <t>UITRGPV_AC_08</t>
-  </si>
-  <si>
-    <t>tr[class='SelectedItem']:nth-of-type(3) a[id*='UCTabs']</t>
-  </si>
-  <si>
-    <t>//ul[@class='list-item']//table[contains(@id, 'UCTabs')]//tr[@class='SelectedItem']//a[contains(@id, 'UCTabs')]</t>
-  </si>
-  <si>
-    <t>tr[class='SelectedItem'] a[id*='UCTabs']</t>
-  </si>
-  <si>
-    <t>a:contains(Proctorial Order September 2023)</t>
-  </si>
-  <si>
-    <t>(//a[contains(text(), 'Proctorial Order September 2023')])[2]</t>
-  </si>
-  <si>
     <t>Demo_QA_01</t>
   </si>
   <si>
@@ -1183,9 +1111,6 @@
     <t>Shubham</t>
   </si>
   <si>
-    <t>UITRGPV_AC_09</t>
-  </si>
-  <si>
     <t>//footer//div[contains(@class, 'col-lg-')][1]//ul[@class='list-item']/i[@class='la la-angle-right'][1]</t>
   </si>
   <si>
@@ -1490,6 +1415,12 @@
   </si>
   <si>
     <t>div[class*='col-lg-']&gt;div[class='footer_col'] ul[class='list-item']&gt;i[class='la la-angle-right']</t>
+  </si>
+  <si>
+    <t>div[class*='col-lg-']:nth-of-type(2) ul[class='list-item']&gt;li:nth-of-type(1)&gt;a</t>
+  </si>
+  <si>
+    <t>div[class*='col-lg-'] ul[class='list-item']&gt;li&gt;a</t>
   </si>
 </sst>
 </file>
@@ -1857,11 +1788,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1006"/>
+  <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I75" sqref="I75"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1943,22 +1874,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>15</v>
@@ -1994,22 +1925,22 @@
         <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>15</v>
@@ -2051,10 +1982,10 @@
         <v>23</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>24</v>
@@ -2090,28 +2021,28 @@
         <v>12</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>478</v>
+        <v>453</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>15</v>
@@ -2147,16 +2078,16 @@
         <v>30</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>31</v>
@@ -2204,16 +2135,16 @@
         <v>38</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>39</v>
@@ -2243,28 +2174,28 @@
         <v>34</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>479</v>
+        <v>454</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>480</v>
+        <v>455</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>15</v>
@@ -2294,22 +2225,22 @@
         <v>34</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>481</v>
+        <v>456</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>482</v>
+        <v>457</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>44</v>
@@ -2357,10 +2288,10 @@
         <v>51</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>52</v>
@@ -2408,10 +2339,10 @@
         <v>51</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>58</v>
@@ -2453,22 +2384,22 @@
         <v>62</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>46</v>
@@ -2498,28 +2429,28 @@
         <v>34</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>483</v>
+        <v>458</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>484</v>
+        <v>459</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>66</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>46</v>
@@ -2561,10 +2492,10 @@
         <v>70</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>71</v>
@@ -2612,10 +2543,10 @@
         <v>77</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>78</v>
@@ -2654,7 +2585,7 @@
         <v>82</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>485</v>
+        <v>460</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>83</v>
@@ -2663,10 +2594,10 @@
         <v>84</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>85</v>
@@ -2702,28 +2633,28 @@
         <v>34</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>486</v>
+        <v>461</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>487</v>
+        <v>462</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>488</v>
+        <v>463</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>489</v>
+        <v>464</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>80</v>
@@ -2759,22 +2690,22 @@
         <v>90</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>91</v>
@@ -2810,16 +2741,16 @@
         <v>94</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>96</v>
@@ -2855,22 +2786,22 @@
         <v>34</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>452</v>
+        <v>427</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>453</v>
+        <v>428</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>99</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>100</v>
@@ -2912,22 +2843,22 @@
         <v>103</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>104</v>
@@ -2960,25 +2891,25 @@
         <v>106</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>450</v>
+        <v>425</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>107</v>
@@ -3008,22 +2939,22 @@
         <v>34</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>448</v>
+        <v>423</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>109</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>110</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>111</v>
@@ -3059,28 +2990,28 @@
         <v>34</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>114</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>446</v>
+        <v>421</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>107</v>
@@ -3110,22 +3041,22 @@
         <v>117</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>425</v>
+        <v>400</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>426</v>
+        <v>401</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>120</v>
@@ -3161,22 +3092,22 @@
         <v>117</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>421</v>
+        <v>396</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>422</v>
+        <v>397</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>423</v>
+        <v>398</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>123</v>
@@ -3212,22 +3143,22 @@
         <v>117</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>427</v>
+        <v>402</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>126</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>127</v>
@@ -3263,28 +3194,28 @@
         <v>117</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>130</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>447</v>
+        <v>422</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>131</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>107</v>
@@ -3314,28 +3245,28 @@
         <v>133</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>134</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>135</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>107</v>
@@ -3365,28 +3296,28 @@
         <v>137</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>429</v>
+        <v>404</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>107</v>
@@ -3416,22 +3347,22 @@
         <v>139</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>140</v>
@@ -3479,10 +3410,10 @@
         <v>147</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>148</v>
@@ -3524,16 +3455,16 @@
         <v>152</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>153</v>
@@ -3569,22 +3500,22 @@
         <v>143</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>156</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>158</v>
@@ -3632,10 +3563,10 @@
         <v>147</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>163</v>
@@ -3671,28 +3602,28 @@
         <v>166</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>167</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>107</v>
@@ -3728,16 +3659,16 @@
         <v>170</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>171</v>
@@ -3779,16 +3710,16 @@
         <v>175</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>176</v>
@@ -3836,10 +3767,10 @@
         <v>182</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>183</v>
@@ -3887,16 +3818,16 @@
         <v>190</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>107</v>
@@ -3926,22 +3857,22 @@
         <v>166</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>432</v>
+        <v>407</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>192</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>433</v>
+        <v>408</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>193</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>194</v>
@@ -3977,22 +3908,22 @@
         <v>166</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>198</v>
@@ -4034,22 +3965,22 @@
         <v>203</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>107</v>
@@ -4079,28 +4010,28 @@
         <v>205</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>430</v>
+        <v>405</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>431</v>
+        <v>406</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>107</v>
@@ -4136,22 +4067,22 @@
         <v>208</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>107</v>
@@ -4184,25 +4115,25 @@
         <v>208</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>434</v>
+        <v>409</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>107</v>
@@ -4238,22 +4169,22 @@
         <v>212</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>107</v>
@@ -4283,28 +4214,28 @@
         <v>207</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>438</v>
+        <v>413</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>442</v>
+        <v>417</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>439</v>
+        <v>414</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>214</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>440</v>
+        <v>415</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>441</v>
+        <v>416</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>107</v>
@@ -4334,24 +4265,24 @@
         <v>207</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>435</v>
+        <v>410</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>436</v>
+        <v>411</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>437</v>
+        <v>412</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>443</v>
+        <v>418</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>107</v>
@@ -4375,30 +4306,30 @@
     </row>
     <row r="50" spans="1:27" ht="66.599999999999994" thickBot="1">
       <c r="A50" s="11" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>445</v>
+        <v>420</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>444</v>
+        <v>419</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50" s="11"/>
@@ -4436,16 +4367,16 @@
         <v>221</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K51" s="5" t="s">
         <v>107</v>
@@ -4487,16 +4418,16 @@
         <v>226</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>107</v>
@@ -4538,10 +4469,10 @@
         <v>231</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>232</v>
@@ -4589,10 +4520,10 @@
         <v>238</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>239</v>
@@ -4601,7 +4532,7 @@
         <v>240</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
@@ -4640,10 +4571,10 @@
         <v>246</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>247</v>
@@ -4685,16 +4616,16 @@
         <v>252</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>253</v>
@@ -4742,10 +4673,10 @@
         <v>260</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>261</v>
@@ -4781,22 +4712,22 @@
         <v>256</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>474</v>
+        <v>449</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>264</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>265</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>266</v>
@@ -4832,22 +4763,22 @@
         <v>269</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>270</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>271</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>272</v>
@@ -4889,22 +4820,22 @@
         <v>276</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K60" s="5" t="s">
         <v>249</v>
@@ -4940,22 +4871,22 @@
         <v>280</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>107</v>
@@ -4991,22 +4922,22 @@
         <v>284</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>285</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K62" s="5" t="s">
         <v>249</v>
@@ -5048,10 +4979,10 @@
         <v>290</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>291</v>
@@ -5099,10 +5030,10 @@
         <v>297</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>298</v>
@@ -5150,10 +5081,10 @@
         <v>304</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>305</v>
@@ -5195,22 +5126,22 @@
         <v>309</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>107</v>
@@ -5232,43 +5163,41 @@
       <c r="Z66" s="6"/>
       <c r="AA66" s="6"/>
     </row>
-    <row r="67" spans="1:27" ht="92.4">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:27" ht="79.2">
+      <c r="A67" s="6" t="s">
         <v>310</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>308</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I67" s="9" t="s">
-        <v>371</v>
-      </c>
-      <c r="J67" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>318</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="L67" s="5" t="s">
-        <v>315</v>
-      </c>
+      <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
@@ -5285,87 +5214,87 @@
       <c r="Z67" s="9"/>
       <c r="AA67" s="9"/>
     </row>
-    <row r="68" spans="1:27" ht="79.2">
-      <c r="A68" s="3" t="s">
-        <v>316</v>
+    <row r="68" spans="1:27" ht="13.2">
+      <c r="A68" s="6" t="s">
+        <v>311</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="F68" s="5" t="s">
+      <c r="C68" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="D68" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>347</v>
+      </c>
       <c r="G68" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I68" s="9" t="s">
-        <v>371</v>
-      </c>
-      <c r="J68" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>347</v>
       </c>
       <c r="K68" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="9"/>
-      <c r="R68" s="9"/>
-      <c r="S68" s="9"/>
-      <c r="T68" s="9"/>
-      <c r="U68" s="9"/>
-      <c r="V68" s="9"/>
-      <c r="W68" s="9"/>
-      <c r="X68" s="9"/>
-      <c r="Y68" s="9"/>
-      <c r="Z68" s="9"/>
-      <c r="AA68" s="9"/>
-    </row>
-    <row r="69" spans="1:27" ht="79.2">
-      <c r="A69" s="3" t="s">
-        <v>321</v>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="6"/>
+      <c r="T68" s="6"/>
+      <c r="U68" s="6"/>
+      <c r="V68" s="6"/>
+      <c r="W68" s="6"/>
+      <c r="X68" s="6"/>
+      <c r="Y68" s="6"/>
+      <c r="Z68" s="6"/>
+      <c r="AA68" s="6"/>
+    </row>
+    <row r="69" spans="1:27" ht="66.599999999999994" thickBot="1">
+      <c r="A69" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="D69" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="E69" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="F69" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="G69" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="I69" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="J69" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>327</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>107</v>
@@ -5387,140 +5316,132 @@
       <c r="Z69" s="9"/>
       <c r="AA69" s="9"/>
     </row>
-    <row r="70" spans="1:27" ht="13.2">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:27" ht="106.2" thickBot="1">
+      <c r="A70" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L70" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+      <c r="P70" s="11"/>
+      <c r="Q70" s="11"/>
+      <c r="R70" s="11"/>
+      <c r="S70" s="11"/>
+      <c r="T70" s="11"/>
+      <c r="U70" s="11"/>
+      <c r="V70" s="11"/>
+      <c r="W70" s="11"/>
+      <c r="X70" s="11"/>
+      <c r="Y70" s="11"/>
+      <c r="Z70" s="11"/>
+      <c r="AA70" s="11"/>
+    </row>
+    <row r="71" spans="1:27" ht="118.8">
+      <c r="A71" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="I71" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C70" s="3" t="s">
+      <c r="J71" s="9" t="s">
         <v>329</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I70" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="J70" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="L70" s="6"/>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="6"/>
-      <c r="P70" s="6"/>
-      <c r="Q70" s="6"/>
-      <c r="R70" s="6"/>
-      <c r="S70" s="6"/>
-      <c r="T70" s="6"/>
-      <c r="U70" s="6"/>
-      <c r="V70" s="6"/>
-      <c r="W70" s="6"/>
-      <c r="X70" s="6"/>
-      <c r="Y70" s="6"/>
-      <c r="Z70" s="6"/>
-      <c r="AA70" s="6"/>
-    </row>
-    <row r="71" spans="1:27" ht="66">
-      <c r="A71" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I71" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>371</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="L71" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
-      <c r="P71" s="6"/>
-      <c r="Q71" s="6"/>
-      <c r="R71" s="6"/>
-      <c r="S71" s="6"/>
-      <c r="T71" s="6"/>
-      <c r="U71" s="6"/>
-      <c r="V71" s="6"/>
-      <c r="W71" s="6"/>
-      <c r="X71" s="6"/>
-      <c r="Y71" s="6"/>
-      <c r="Z71" s="6"/>
-      <c r="AA71" s="6"/>
-    </row>
-    <row r="72" spans="1:27" ht="66">
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="9"/>
+      <c r="R71" s="9"/>
+      <c r="S71" s="9"/>
+      <c r="T71" s="9"/>
+      <c r="U71" s="9"/>
+      <c r="V71" s="9"/>
+      <c r="W71" s="9"/>
+      <c r="X71" s="9"/>
+      <c r="Y71" s="9"/>
+      <c r="Z71" s="9"/>
+      <c r="AA71" s="9"/>
+    </row>
+    <row r="72" spans="1:27" ht="39.6">
       <c r="A72" s="5" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>341</v>
+        <v>331</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>333</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>343</v>
+        <v>347</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="J72" s="9" t="s">
+        <v>335</v>
       </c>
       <c r="K72" s="5" t="s">
         <v>107</v>
@@ -5542,36 +5463,36 @@
       <c r="Z72" s="9"/>
       <c r="AA72" s="9"/>
     </row>
-    <row r="73" spans="1:27" ht="106.2" thickBot="1">
+    <row r="73" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A73" s="5" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>345</v>
+        <v>327</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>337</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>347</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>51</v>
+        <v>347</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="K73" s="5" t="s">
         <v>107</v>
@@ -5593,34 +5514,38 @@
       <c r="Z73" s="9"/>
       <c r="AA73" s="9"/>
     </row>
-    <row r="74" spans="1:27" ht="106.2" thickBot="1">
+    <row r="74" spans="1:27" ht="145.80000000000001" thickBot="1">
       <c r="A74" s="11" t="s">
-        <v>389</v>
+        <v>368</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>308</v>
+        <v>369</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>491</v>
+        <v>448</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
+      <c r="I74" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="J74" s="11" t="s">
+        <v>373</v>
+      </c>
       <c r="K74" s="11" t="s">
         <v>107</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>392</v>
+        <v>367</v>
       </c>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
@@ -5638,87 +5563,85 @@
       <c r="Z74" s="11"/>
       <c r="AA74" s="11"/>
     </row>
-    <row r="75" spans="1:27" ht="118.8">
-      <c r="A75" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>467</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>468</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I75" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="J75" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="K75" s="5" t="s">
+    <row r="75" spans="1:27" ht="27" thickBot="1">
+      <c r="A75" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="J75" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="K75" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
-      <c r="P75" s="9"/>
-      <c r="Q75" s="9"/>
-      <c r="R75" s="9"/>
-      <c r="S75" s="9"/>
-      <c r="T75" s="9"/>
-      <c r="U75" s="9"/>
-      <c r="V75" s="9"/>
-      <c r="W75" s="9"/>
-      <c r="X75" s="9"/>
-      <c r="Y75" s="9"/>
-      <c r="Z75" s="9"/>
-      <c r="AA75" s="9"/>
-    </row>
-    <row r="76" spans="1:27" ht="39.6">
-      <c r="A76" s="5" t="s">
-        <v>354</v>
+      <c r="L75" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="M75" s="11"/>
+      <c r="N75" s="11"/>
+      <c r="O75" s="11"/>
+      <c r="P75" s="11"/>
+      <c r="Q75" s="11"/>
+      <c r="R75" s="11"/>
+      <c r="S75" s="11"/>
+      <c r="T75" s="11"/>
+      <c r="U75" s="11"/>
+      <c r="V75" s="11"/>
+      <c r="W75" s="11"/>
+      <c r="X75" s="11"/>
+      <c r="Y75" s="11"/>
+      <c r="Z75" s="11"/>
+      <c r="AA75" s="11"/>
+    </row>
+    <row r="76" spans="1:27" ht="66.599999999999994" thickBot="1">
+      <c r="A76" s="9" t="s">
+        <v>341</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>470</v>
+        <v>429</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>471</v>
+        <v>430</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>107</v>
@@ -5741,88 +5664,86 @@
       <c r="AA76" s="9"/>
     </row>
     <row r="77" spans="1:27" ht="40.200000000000003" thickBot="1">
-      <c r="A77" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="K77" s="5" t="s">
+      <c r="A77" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="F77" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="J77" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="K77" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="9"/>
-      <c r="O77" s="9"/>
-      <c r="P77" s="9"/>
-      <c r="Q77" s="9"/>
-      <c r="R77" s="9"/>
-      <c r="S77" s="9"/>
-      <c r="T77" s="9"/>
-      <c r="U77" s="9"/>
-      <c r="V77" s="9"/>
-      <c r="W77" s="9"/>
-      <c r="X77" s="9"/>
-      <c r="Y77" s="9"/>
-      <c r="Z77" s="9"/>
-      <c r="AA77" s="9"/>
-    </row>
-    <row r="78" spans="1:27" ht="145.80000000000001" thickBot="1">
+      <c r="L77" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="M77" s="11"/>
+      <c r="N77" s="11"/>
+      <c r="O77" s="11"/>
+      <c r="P77" s="11"/>
+      <c r="Q77" s="11"/>
+      <c r="R77" s="11"/>
+      <c r="S77" s="11"/>
+      <c r="T77" s="11"/>
+      <c r="U77" s="11"/>
+      <c r="V77" s="11"/>
+      <c r="W77" s="11"/>
+      <c r="X77" s="11"/>
+      <c r="Y77" s="11"/>
+      <c r="Z77" s="11"/>
+      <c r="AA77" s="11"/>
+    </row>
+    <row r="78" spans="1:27" ht="93" thickBot="1">
       <c r="A78" s="11" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>472</v>
+        <v>433</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>473</v>
+        <v>435</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>396</v>
+        <v>436</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11" t="s">
-        <v>397</v>
+        <v>437</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>398</v>
+        <v>438</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>107</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>392</v>
+        <v>367</v>
       </c>
       <c r="M78" s="11"/>
       <c r="N78" s="11"/>
@@ -5842,36 +5763,28 @@
     </row>
     <row r="79" spans="1:27" ht="27" thickBot="1">
       <c r="A79" s="11" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="E79" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="F79" s="11" t="s">
-        <v>404</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
-      <c r="I79" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="J79" s="11" t="s">
-        <v>406</v>
-      </c>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
       <c r="K79" s="11" t="s">
-        <v>107</v>
+        <v>249</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>392</v>
+        <v>367</v>
       </c>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
@@ -5890,243 +5803,169 @@
       <c r="AA79" s="11"/>
     </row>
     <row r="80" spans="1:27" ht="66.599999999999994" thickBot="1">
-      <c r="A80" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="D80" s="9" t="s">
+      <c r="A80" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="J80" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="K80" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L80" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="E80" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="I80" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="J80" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="K80" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="L80" s="9"/>
-      <c r="M80" s="9"/>
-      <c r="N80" s="9"/>
-      <c r="O80" s="9"/>
-      <c r="P80" s="9"/>
-      <c r="Q80" s="9"/>
-      <c r="R80" s="9"/>
-      <c r="S80" s="9"/>
-      <c r="T80" s="9"/>
-      <c r="U80" s="9"/>
-      <c r="V80" s="9"/>
-      <c r="W80" s="9"/>
-      <c r="X80" s="9"/>
-      <c r="Y80" s="9"/>
-      <c r="Z80" s="9"/>
-      <c r="AA80" s="9"/>
-    </row>
-    <row r="81" spans="1:27" ht="40.200000000000003" thickBot="1">
-      <c r="A81" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>457</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="F81" s="13" t="s">
-        <v>408</v>
-      </c>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="J81" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="K81" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L81" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="M81" s="11"/>
-      <c r="N81" s="11"/>
-      <c r="O81" s="11"/>
-      <c r="P81" s="11"/>
-      <c r="Q81" s="11"/>
-      <c r="R81" s="11"/>
-      <c r="S81" s="11"/>
-      <c r="T81" s="11"/>
-      <c r="U81" s="11"/>
-      <c r="V81" s="11"/>
-      <c r="W81" s="11"/>
-      <c r="X81" s="11"/>
-      <c r="Y81" s="11"/>
-      <c r="Z81" s="11"/>
-      <c r="AA81" s="11"/>
-    </row>
-    <row r="82" spans="1:27" ht="93" thickBot="1">
-      <c r="A82" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="F82" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="J82" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="K82" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L82" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="M82" s="11"/>
-      <c r="N82" s="11"/>
-      <c r="O82" s="11"/>
-      <c r="P82" s="11"/>
-      <c r="Q82" s="11"/>
-      <c r="R82" s="11"/>
-      <c r="S82" s="11"/>
-      <c r="T82" s="11"/>
-      <c r="U82" s="11"/>
-      <c r="V82" s="11"/>
-      <c r="W82" s="11"/>
-      <c r="X82" s="11"/>
-      <c r="Y82" s="11"/>
-      <c r="Z82" s="11"/>
-      <c r="AA82" s="11"/>
-    </row>
-    <row r="83" spans="1:27" ht="27" thickBot="1">
-      <c r="A83" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="L83" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="M83" s="11"/>
-      <c r="N83" s="11"/>
-      <c r="O83" s="11"/>
-      <c r="P83" s="11"/>
-      <c r="Q83" s="11"/>
-      <c r="R83" s="11"/>
-      <c r="S83" s="11"/>
-      <c r="T83" s="11"/>
-      <c r="U83" s="11"/>
-      <c r="V83" s="11"/>
-      <c r="W83" s="11"/>
-      <c r="X83" s="11"/>
-      <c r="Y83" s="11"/>
-      <c r="Z83" s="11"/>
-      <c r="AA83" s="11"/>
-    </row>
-    <row r="84" spans="1:27" ht="66.599999999999994" thickBot="1">
-      <c r="A84" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>464</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="J84" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="K84" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L84" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="M84" s="11"/>
-      <c r="N84" s="11"/>
-      <c r="O84" s="11"/>
-      <c r="P84" s="11"/>
-      <c r="Q84" s="11"/>
-      <c r="R84" s="11"/>
-      <c r="S84" s="11"/>
-      <c r="T84" s="11"/>
-      <c r="U84" s="11"/>
-      <c r="V84" s="11"/>
-      <c r="W84" s="11"/>
-      <c r="X84" s="11"/>
-      <c r="Y84" s="11"/>
-      <c r="Z84" s="11"/>
-      <c r="AA84" s="11"/>
+      <c r="M80" s="11"/>
+      <c r="N80" s="11"/>
+      <c r="O80" s="11"/>
+      <c r="P80" s="11"/>
+      <c r="Q80" s="11"/>
+      <c r="R80" s="11"/>
+      <c r="S80" s="11"/>
+      <c r="T80" s="11"/>
+      <c r="U80" s="11"/>
+      <c r="V80" s="11"/>
+      <c r="W80" s="11"/>
+      <c r="X80" s="11"/>
+      <c r="Y80" s="11"/>
+      <c r="Z80" s="11"/>
+      <c r="AA80" s="11"/>
+    </row>
+    <row r="81" spans="1:27" ht="13.2">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
+      <c r="Q81" s="6"/>
+      <c r="R81" s="6"/>
+      <c r="S81" s="6"/>
+      <c r="T81" s="6"/>
+      <c r="U81" s="6"/>
+      <c r="V81" s="6"/>
+      <c r="W81" s="6"/>
+      <c r="X81" s="6"/>
+      <c r="Y81" s="6"/>
+      <c r="Z81" s="6"/>
+      <c r="AA81" s="6"/>
+    </row>
+    <row r="82" spans="1:27" ht="13.2">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="6"/>
+      <c r="T82" s="6"/>
+      <c r="U82" s="6"/>
+      <c r="V82" s="6"/>
+      <c r="W82" s="6"/>
+      <c r="X82" s="6"/>
+      <c r="Y82" s="6"/>
+      <c r="Z82" s="6"/>
+      <c r="AA82" s="6"/>
+    </row>
+    <row r="83" spans="1:27" ht="13.2">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="6"/>
+      <c r="T83" s="6"/>
+      <c r="U83" s="6"/>
+      <c r="V83" s="6"/>
+      <c r="W83" s="6"/>
+      <c r="X83" s="6"/>
+      <c r="Y83" s="6"/>
+      <c r="Z83" s="6"/>
+      <c r="AA83" s="6"/>
+    </row>
+    <row r="84" spans="1:27" ht="13.2">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="6"/>
+      <c r="Q84" s="6"/>
+      <c r="R84" s="6"/>
+      <c r="S84" s="6"/>
+      <c r="T84" s="6"/>
+      <c r="U84" s="6"/>
+      <c r="V84" s="6"/>
+      <c r="W84" s="6"/>
+      <c r="X84" s="6"/>
+      <c r="Y84" s="6"/>
+      <c r="Z84" s="6"/>
+      <c r="AA84" s="6"/>
     </row>
     <row r="85" spans="1:27" ht="13.2">
       <c r="A85" s="6"/>
@@ -32749,122 +32588,6 @@
       <c r="Y1002" s="6"/>
       <c r="Z1002" s="6"/>
       <c r="AA1002" s="6"/>
-    </row>
-    <row r="1003" spans="1:27" ht="13.2">
-      <c r="A1003" s="6"/>
-      <c r="B1003" s="6"/>
-      <c r="C1003" s="6"/>
-      <c r="D1003" s="6"/>
-      <c r="E1003" s="6"/>
-      <c r="F1003" s="6"/>
-      <c r="G1003" s="6"/>
-      <c r="H1003" s="6"/>
-      <c r="I1003" s="6"/>
-      <c r="J1003" s="6"/>
-      <c r="K1003" s="6"/>
-      <c r="L1003" s="6"/>
-      <c r="M1003" s="6"/>
-      <c r="N1003" s="6"/>
-      <c r="O1003" s="6"/>
-      <c r="P1003" s="6"/>
-      <c r="Q1003" s="6"/>
-      <c r="R1003" s="6"/>
-      <c r="S1003" s="6"/>
-      <c r="T1003" s="6"/>
-      <c r="U1003" s="6"/>
-      <c r="V1003" s="6"/>
-      <c r="W1003" s="6"/>
-      <c r="X1003" s="6"/>
-      <c r="Y1003" s="6"/>
-      <c r="Z1003" s="6"/>
-      <c r="AA1003" s="6"/>
-    </row>
-    <row r="1004" spans="1:27" ht="13.2">
-      <c r="A1004" s="6"/>
-      <c r="B1004" s="6"/>
-      <c r="C1004" s="6"/>
-      <c r="D1004" s="6"/>
-      <c r="E1004" s="6"/>
-      <c r="F1004" s="6"/>
-      <c r="G1004" s="6"/>
-      <c r="H1004" s="6"/>
-      <c r="I1004" s="6"/>
-      <c r="J1004" s="6"/>
-      <c r="K1004" s="6"/>
-      <c r="L1004" s="6"/>
-      <c r="M1004" s="6"/>
-      <c r="N1004" s="6"/>
-      <c r="O1004" s="6"/>
-      <c r="P1004" s="6"/>
-      <c r="Q1004" s="6"/>
-      <c r="R1004" s="6"/>
-      <c r="S1004" s="6"/>
-      <c r="T1004" s="6"/>
-      <c r="U1004" s="6"/>
-      <c r="V1004" s="6"/>
-      <c r="W1004" s="6"/>
-      <c r="X1004" s="6"/>
-      <c r="Y1004" s="6"/>
-      <c r="Z1004" s="6"/>
-      <c r="AA1004" s="6"/>
-    </row>
-    <row r="1005" spans="1:27" ht="13.2">
-      <c r="A1005" s="6"/>
-      <c r="B1005" s="6"/>
-      <c r="C1005" s="6"/>
-      <c r="D1005" s="6"/>
-      <c r="E1005" s="6"/>
-      <c r="F1005" s="6"/>
-      <c r="G1005" s="6"/>
-      <c r="H1005" s="6"/>
-      <c r="I1005" s="6"/>
-      <c r="J1005" s="6"/>
-      <c r="K1005" s="6"/>
-      <c r="L1005" s="6"/>
-      <c r="M1005" s="6"/>
-      <c r="N1005" s="6"/>
-      <c r="O1005" s="6"/>
-      <c r="P1005" s="6"/>
-      <c r="Q1005" s="6"/>
-      <c r="R1005" s="6"/>
-      <c r="S1005" s="6"/>
-      <c r="T1005" s="6"/>
-      <c r="U1005" s="6"/>
-      <c r="V1005" s="6"/>
-      <c r="W1005" s="6"/>
-      <c r="X1005" s="6"/>
-      <c r="Y1005" s="6"/>
-      <c r="Z1005" s="6"/>
-      <c r="AA1005" s="6"/>
-    </row>
-    <row r="1006" spans="1:27" ht="13.2">
-      <c r="A1006" s="6"/>
-      <c r="B1006" s="6"/>
-      <c r="C1006" s="6"/>
-      <c r="D1006" s="6"/>
-      <c r="E1006" s="6"/>
-      <c r="F1006" s="6"/>
-      <c r="G1006" s="6"/>
-      <c r="H1006" s="6"/>
-      <c r="I1006" s="6"/>
-      <c r="J1006" s="6"/>
-      <c r="K1006" s="6"/>
-      <c r="L1006" s="6"/>
-      <c r="M1006" s="6"/>
-      <c r="N1006" s="6"/>
-      <c r="O1006" s="6"/>
-      <c r="P1006" s="6"/>
-      <c r="Q1006" s="6"/>
-      <c r="R1006" s="6"/>
-      <c r="S1006" s="6"/>
-      <c r="T1006" s="6"/>
-      <c r="U1006" s="6"/>
-      <c r="V1006" s="6"/>
-      <c r="W1006" s="6"/>
-      <c r="X1006" s="6"/>
-      <c r="Y1006" s="6"/>
-      <c r="Z1006" s="6"/>
-      <c r="AA1006" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -32934,24 +32657,20 @@
     <hyperlink ref="B67" r:id="rId64"/>
     <hyperlink ref="B68" r:id="rId65"/>
     <hyperlink ref="B69" r:id="rId66"/>
-    <hyperlink ref="B70" r:id="rId67"/>
-    <hyperlink ref="B71" r:id="rId68"/>
-    <hyperlink ref="B72" r:id="rId69"/>
-    <hyperlink ref="B73" r:id="rId70"/>
-    <hyperlink ref="B75" r:id="rId71"/>
-    <hyperlink ref="B76" r:id="rId72"/>
-    <hyperlink ref="B77" r:id="rId73"/>
-    <hyperlink ref="B80" r:id="rId74"/>
-    <hyperlink ref="B50" r:id="rId75"/>
-    <hyperlink ref="B74" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78" display="https://demoqa.com/menu"/>
-    <hyperlink ref="B81" r:id="rId79"/>
-    <hyperlink ref="B82" r:id="rId80"/>
-    <hyperlink ref="B83" r:id="rId81"/>
-    <hyperlink ref="B84" r:id="rId82"/>
+    <hyperlink ref="B71" r:id="rId67"/>
+    <hyperlink ref="B72" r:id="rId68"/>
+    <hyperlink ref="B73" r:id="rId69"/>
+    <hyperlink ref="B76" r:id="rId70"/>
+    <hyperlink ref="B50" r:id="rId71"/>
+    <hyperlink ref="B70" r:id="rId72"/>
+    <hyperlink ref="B74" r:id="rId73"/>
+    <hyperlink ref="B75" r:id="rId74" display="https://demoqa.com/menu"/>
+    <hyperlink ref="B77" r:id="rId75"/>
+    <hyperlink ref="B78" r:id="rId76"/>
+    <hyperlink ref="B79" r:id="rId77"/>
+    <hyperlink ref="B80" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId83"/>
+  <pageSetup orientation="portrait" r:id="rId79"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test case in rgpv
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="510">
   <si>
     <t>ID</t>
   </si>
@@ -1538,6 +1538,12 @@
   </si>
   <si>
     <t>p[class='footer-text copyright']:nth-of-type(1) &gt; a:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>//button[@class='btn-close']</t>
+  </si>
+  <si>
+    <t>Iframe</t>
   </si>
 </sst>
 </file>
@@ -1908,8 +1914,8 @@
   <dimension ref="A1:AA1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4387,8 +4393,12 @@
       <c r="D49" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>385</v>
+      </c>
       <c r="G49" s="6" t="s">
         <v>385</v>
       </c>
@@ -4434,17 +4444,27 @@
       <c r="D50" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="E50" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>385</v>
+      </c>
       <c r="G50" s="11" t="s">
         <v>400</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
+      <c r="I50" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>509</v>
+      </c>
       <c r="L50" s="11" t="s">
         <v>402</v>
       </c>
@@ -5240,7 +5260,7 @@
         <v>315</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>315</v>
+        <v>508</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>385</v>
@@ -33141,29 +33161,29 @@
     <hyperlink ref="B64" r:id="rId61"/>
     <hyperlink ref="B65" r:id="rId62"/>
     <hyperlink ref="B66" r:id="rId63"/>
-    <hyperlink ref="B67" r:id="rId64"/>
-    <hyperlink ref="B68" r:id="rId65"/>
-    <hyperlink ref="B69" r:id="rId66"/>
-    <hyperlink ref="B70" r:id="rId67"/>
-    <hyperlink ref="B71" r:id="rId68"/>
-    <hyperlink ref="B72" r:id="rId69"/>
-    <hyperlink ref="B73" r:id="rId70"/>
-    <hyperlink ref="B75" r:id="rId71"/>
-    <hyperlink ref="B76" r:id="rId72"/>
-    <hyperlink ref="B77" r:id="rId73"/>
-    <hyperlink ref="B80" r:id="rId74"/>
-    <hyperlink ref="B50" r:id="rId75"/>
-    <hyperlink ref="B74" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78" display="https://demoqa.com/menu"/>
-    <hyperlink ref="B81" r:id="rId79"/>
-    <hyperlink ref="B82" r:id="rId80"/>
-    <hyperlink ref="B83" r:id="rId81"/>
-    <hyperlink ref="B84" r:id="rId82"/>
-    <hyperlink ref="B85" r:id="rId83"/>
-    <hyperlink ref="B86" r:id="rId84"/>
-    <hyperlink ref="B87" r:id="rId85"/>
-    <hyperlink ref="B88" r:id="rId86"/>
+    <hyperlink ref="B68" r:id="rId64"/>
+    <hyperlink ref="B69" r:id="rId65"/>
+    <hyperlink ref="B70" r:id="rId66"/>
+    <hyperlink ref="B71" r:id="rId67"/>
+    <hyperlink ref="B72" r:id="rId68"/>
+    <hyperlink ref="B73" r:id="rId69"/>
+    <hyperlink ref="B75" r:id="rId70"/>
+    <hyperlink ref="B76" r:id="rId71"/>
+    <hyperlink ref="B77" r:id="rId72"/>
+    <hyperlink ref="B80" r:id="rId73"/>
+    <hyperlink ref="B50" r:id="rId74"/>
+    <hyperlink ref="B74" r:id="rId75"/>
+    <hyperlink ref="B78" r:id="rId76"/>
+    <hyperlink ref="B79" r:id="rId77" display="https://demoqa.com/menu"/>
+    <hyperlink ref="B81" r:id="rId78"/>
+    <hyperlink ref="B82" r:id="rId79"/>
+    <hyperlink ref="B83" r:id="rId80"/>
+    <hyperlink ref="B84" r:id="rId81"/>
+    <hyperlink ref="B85" r:id="rId82"/>
+    <hyperlink ref="B86" r:id="rId83"/>
+    <hyperlink ref="B87" r:id="rId84"/>
+    <hyperlink ref="B88" r:id="rId85"/>
+    <hyperlink ref="B67" r:id="rId86"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId87"/>

</xml_diff>

<commit_message>
updated manual test case
</commit_message>
<xml_diff>
--- a/src/main/resources/FML_LocatorSheet.xlsx
+++ b/src/main/resources/FML_LocatorSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="542">
   <si>
     <t>ID</t>
   </si>
@@ -1526,6 +1526,120 @@
   </si>
   <si>
     <t>Iframe_Tosca_02</t>
+  </si>
+  <si>
+    <t>indiapost_TC_01</t>
+  </si>
+  <si>
+    <t>https://www.indiapost.gov.in/vas/Pages/IndiaPostHome.aspx</t>
+  </si>
+  <si>
+    <t>img[id='india-post-logo']</t>
+  </si>
+  <si>
+    <t>//img[@id='india-post-logo']</t>
+  </si>
+  <si>
+    <t>indiapost_TC_02</t>
+  </si>
+  <si>
+    <t>img[id='emblem-of-india-logo']</t>
+  </si>
+  <si>
+    <t>//img[@id='emblem-of-india-logo']</t>
+  </si>
+  <si>
+    <t>left click</t>
+  </si>
+  <si>
+    <t>indiapost_TC_03</t>
+  </si>
+  <si>
+    <t>img[alt*='Web']</t>
+  </si>
+  <si>
+    <t>//img[contains(@alt, 'Web')]</t>
+  </si>
+  <si>
+    <t>indiapost_TC_04</t>
+  </si>
+  <si>
+    <t>img[id='feature-box-item-image/']</t>
+  </si>
+  <si>
+    <t>//img[@id='feature-box-item-image/']</t>
+  </si>
+  <si>
+    <t>indiapost_TC_05</t>
+  </si>
+  <si>
+    <t>label[class='control-label radio-inline']:nth-of-type(3) &gt; input[id*='ctl']</t>
+  </si>
+  <si>
+    <t>//label[@class='control-label radio-inline'][2]/input[contains(@id, 'ctl')]</t>
+  </si>
+  <si>
+    <t>label[class='control-label radio-inline'] &gt; input[id*='ctl']</t>
+  </si>
+  <si>
+    <t>//label[@class='control-label radio-inline']/input[contains(@id, 'ctl')]</t>
+  </si>
+  <si>
+    <t>indiapost_TC_06</t>
+  </si>
+  <si>
+    <t>input[aria-label='Enter a valid complaint number']</t>
+  </si>
+  <si>
+    <t>//input[@aria-label='Enter a valid complaint number']</t>
+  </si>
+  <si>
+    <t>indiapost_TC_07</t>
+  </si>
+  <si>
+    <t>img[id*='ctl']</t>
+  </si>
+  <si>
+    <t>//img[contains(@id, 'ctl')]</t>
+  </si>
+  <si>
+    <t>indiapost_TC_08</t>
+  </si>
+  <si>
+    <t>input[class*='btn']</t>
+  </si>
+  <si>
+    <t>//input[contains(@class, 'btn')]</t>
+  </si>
+  <si>
+    <t>indiapost_TC_09</t>
+  </si>
+  <si>
+    <t>div[id='feature-box-item-helpline'] &gt; h4:nth-of-type(1)</t>
+  </si>
+  <si>
+    <t>//div[@id='feature-box-item-helpline']/h4[1]</t>
+  </si>
+  <si>
+    <t>div[id='feature-box-item-helpline'] &gt; h4</t>
+  </si>
+  <si>
+    <t>//div[@id='feature-box-item-helpline']/h4</t>
+  </si>
+  <si>
+    <t>h4:contains(Toll Free Enquiry Helpline:)</t>
+  </si>
+  <si>
+    <t>//h4[contains(text(), 'Toll Free Enquiry Helpline:')]</t>
+  </si>
+  <si>
+    <t>indiapost_TC_10</t>
+  </si>
+  <si>
+    <t>img[alt='Calculate Postage']</t>
+  </si>
+  <si>
+    <t>//img[@alt='Calculate Postage']</t>
   </si>
 </sst>
 </file>
@@ -1656,7 +1770,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1714,6 +1828,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1934,7 +2051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
+      <selection pane="bottomLeft" activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1942,13 +2059,13 @@
     <col min="1" max="1" width="51" customWidth="1"/>
     <col min="2" max="2" width="39.77734375" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" customWidth="1"/>
     <col min="8" max="8" width="19.21875" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="41.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="13.8">
@@ -2002,7 +2119,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="79.2">
+    <row r="2" spans="1:27" ht="52.8">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -2053,7 +2170,7 @@
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
     </row>
-    <row r="3" spans="1:27" ht="79.2">
+    <row r="3" spans="1:27" ht="52.8">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -2104,7 +2221,7 @@
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
     </row>
-    <row r="4" spans="1:27" ht="92.4">
+    <row r="4" spans="1:27" ht="82.8">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -2155,7 +2272,7 @@
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
     </row>
-    <row r="5" spans="1:27" ht="79.2">
+    <row r="5" spans="1:27" ht="52.8">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -2206,7 +2323,7 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
     </row>
-    <row r="6" spans="1:27" ht="39.6">
+    <row r="6" spans="1:27" ht="26.4">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -2257,7 +2374,7 @@
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
     </row>
-    <row r="7" spans="1:27" ht="158.4">
+    <row r="7" spans="1:27" ht="105.6">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -2308,7 +2425,7 @@
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
     </row>
-    <row r="8" spans="1:27" ht="79.2">
+    <row r="8" spans="1:27" ht="52.8">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -2359,7 +2476,7 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
     </row>
-    <row r="9" spans="1:27" ht="158.4">
+    <row r="9" spans="1:27" ht="118.8">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -2410,7 +2527,7 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
     </row>
-    <row r="10" spans="1:27" ht="105.6">
+    <row r="10" spans="1:27" ht="39.6">
       <c r="A10" s="3" t="s">
         <v>47</v>
       </c>
@@ -2461,7 +2578,7 @@
       <c r="Z10" s="6"/>
       <c r="AA10" s="6"/>
     </row>
-    <row r="11" spans="1:27" ht="105.6">
+    <row r="11" spans="1:27" ht="52.8">
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
@@ -2512,7 +2629,7 @@
       <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
     </row>
-    <row r="12" spans="1:27" ht="39.6">
+    <row r="12" spans="1:27" ht="26.4">
       <c r="A12" s="5" t="s">
         <v>60</v>
       </c>
@@ -2563,7 +2680,7 @@
       <c r="Z12" s="9"/>
       <c r="AA12" s="9"/>
     </row>
-    <row r="13" spans="1:27" ht="105.6">
+    <row r="13" spans="1:27" ht="92.4">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -2614,7 +2731,7 @@
       <c r="Z13" s="9"/>
       <c r="AA13" s="9"/>
     </row>
-    <row r="14" spans="1:27" ht="118.8">
+    <row r="14" spans="1:27" ht="92.4">
       <c r="A14" s="5" t="s">
         <v>67</v>
       </c>
@@ -2665,7 +2782,7 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
     </row>
-    <row r="15" spans="1:27" ht="158.4">
+    <row r="15" spans="1:27" ht="118.8">
       <c r="A15" s="5" t="s">
         <v>73</v>
       </c>
@@ -2716,7 +2833,7 @@
       <c r="Z15" s="9"/>
       <c r="AA15" s="9"/>
     </row>
-    <row r="16" spans="1:27" ht="105.6">
+    <row r="16" spans="1:27" ht="92.4">
       <c r="A16" s="5" t="s">
         <v>81</v>
       </c>
@@ -2767,7 +2884,7 @@
       <c r="Z16" s="9"/>
       <c r="AA16" s="9"/>
     </row>
-    <row r="17" spans="1:27" ht="132">
+    <row r="17" spans="1:27" ht="105.6">
       <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
@@ -2818,7 +2935,7 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
     </row>
-    <row r="18" spans="1:27" ht="105.6">
+    <row r="18" spans="1:27" ht="52.8">
       <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
@@ -2869,7 +2986,7 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
     </row>
-    <row r="19" spans="1:27" ht="145.19999999999999">
+    <row r="19" spans="1:27" ht="118.8">
       <c r="A19" s="5" t="s">
         <v>92</v>
       </c>
@@ -2920,7 +3037,7 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
     </row>
-    <row r="20" spans="1:27" ht="92.4">
+    <row r="20" spans="1:27" ht="79.2">
       <c r="A20" s="5" t="s">
         <v>98</v>
       </c>
@@ -2971,7 +3088,7 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
     </row>
-    <row r="21" spans="1:27" ht="39.6">
+    <row r="21" spans="1:27" ht="26.4">
       <c r="A21" s="5" t="s">
         <v>102</v>
       </c>
@@ -3022,7 +3139,7 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
     </row>
-    <row r="22" spans="1:27" ht="52.8">
+    <row r="22" spans="1:27" ht="26.4">
       <c r="A22" s="5" t="s">
         <v>105</v>
       </c>
@@ -3073,7 +3190,7 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
     </row>
-    <row r="23" spans="1:27" ht="52.8">
+    <row r="23" spans="1:27" ht="39.6">
       <c r="A23" s="5" t="s">
         <v>108</v>
       </c>
@@ -3124,7 +3241,7 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
     </row>
-    <row r="24" spans="1:27" ht="145.80000000000001" thickBot="1">
+    <row r="24" spans="1:27" ht="119.4" thickBot="1">
       <c r="A24" s="15" t="s">
         <v>455</v>
       </c>
@@ -3222,7 +3339,7 @@
       <c r="Z25" s="11"/>
       <c r="AA25" s="11"/>
     </row>
-    <row r="26" spans="1:27" ht="66">
+    <row r="26" spans="1:27" ht="39.6">
       <c r="A26" s="5" t="s">
         <v>115</v>
       </c>
@@ -3273,7 +3390,7 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
     </row>
-    <row r="27" spans="1:27" ht="66">
+    <row r="27" spans="1:27" ht="52.8">
       <c r="A27" s="5" t="s">
         <v>121</v>
       </c>
@@ -3324,7 +3441,7 @@
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
     </row>
-    <row r="28" spans="1:27" ht="66">
+    <row r="28" spans="1:27" ht="52.8">
       <c r="A28" s="5" t="s">
         <v>124</v>
       </c>
@@ -3375,7 +3492,7 @@
       <c r="Z28" s="9"/>
       <c r="AA28" s="9"/>
     </row>
-    <row r="29" spans="1:27" ht="39.6">
+    <row r="29" spans="1:27" ht="26.4">
       <c r="A29" s="5" t="s">
         <v>128</v>
       </c>
@@ -3528,7 +3645,7 @@
       <c r="Z31" s="6"/>
       <c r="AA31" s="6"/>
     </row>
-    <row r="32" spans="1:27" ht="66">
+    <row r="32" spans="1:27" ht="52.8">
       <c r="A32" s="5" t="s">
         <v>137</v>
       </c>
@@ -3579,7 +3696,7 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="5"/>
     </row>
-    <row r="33" spans="1:27" ht="92.4">
+    <row r="33" spans="1:27" ht="79.2">
       <c r="A33" s="5" t="s">
         <v>141</v>
       </c>
@@ -3732,7 +3849,7 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
     </row>
-    <row r="36" spans="1:27" ht="92.4">
+    <row r="36" spans="1:27" ht="79.2">
       <c r="A36" s="5" t="s">
         <v>159</v>
       </c>
@@ -3783,7 +3900,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
     </row>
-    <row r="37" spans="1:27" ht="26.4">
+    <row r="37" spans="1:27" ht="13.2">
       <c r="A37" s="3" t="s">
         <v>164</v>
       </c>
@@ -3885,7 +4002,7 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
     </row>
-    <row r="39" spans="1:27" ht="66">
+    <row r="39" spans="1:27" ht="39.6">
       <c r="A39" s="3" t="s">
         <v>172</v>
       </c>
@@ -3987,7 +4104,7 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
     </row>
-    <row r="41" spans="1:27" ht="66">
+    <row r="41" spans="1:27" ht="52.8">
       <c r="A41" s="3" t="s">
         <v>184</v>
       </c>
@@ -4140,7 +4257,7 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
     </row>
-    <row r="44" spans="1:27" ht="52.8">
+    <row r="44" spans="1:27" ht="39.6">
       <c r="A44" s="3" t="s">
         <v>199</v>
       </c>
@@ -4242,7 +4359,7 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
     </row>
-    <row r="46" spans="1:27" ht="26.4">
+    <row r="46" spans="1:27" ht="13.2">
       <c r="A46" s="3" t="s">
         <v>205</v>
       </c>
@@ -4293,7 +4410,7 @@
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
     </row>
-    <row r="47" spans="1:27" ht="39.6">
+    <row r="47" spans="1:27" ht="13.2">
       <c r="A47" s="3" t="s">
         <v>208</v>
       </c>
@@ -4344,7 +4461,7 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
     </row>
-    <row r="48" spans="1:27" ht="39.6">
+    <row r="48" spans="1:27" ht="26.4">
       <c r="A48" s="3" t="s">
         <v>209</v>
       </c>
@@ -4395,7 +4512,7 @@
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
     </row>
-    <row r="49" spans="1:27" ht="118.8">
+    <row r="49" spans="1:27" ht="92.4">
       <c r="A49" s="3" t="s">
         <v>212</v>
       </c>
@@ -4446,7 +4563,7 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
     </row>
-    <row r="50" spans="1:27" ht="66.599999999999994" thickBot="1">
+    <row r="50" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>214</v>
       </c>
@@ -4493,7 +4610,7 @@
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
     </row>
-    <row r="51" spans="1:27" ht="66.599999999999994" thickBot="1">
+    <row r="51" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A51" s="11" t="s">
         <v>346</v>
       </c>
@@ -4536,7 +4653,7 @@
       <c r="Z51" s="11"/>
       <c r="AA51" s="11"/>
     </row>
-    <row r="52" spans="1:27" ht="79.8" thickBot="1">
+    <row r="52" spans="1:27" ht="40.200000000000003" thickBot="1">
       <c r="A52" s="11" t="s">
         <v>453</v>
       </c>
@@ -4581,7 +4698,7 @@
       <c r="Z52" s="11"/>
       <c r="AA52" s="11"/>
     </row>
-    <row r="53" spans="1:27" ht="79.2">
+    <row r="53" spans="1:27" ht="52.8">
       <c r="A53" s="3" t="s">
         <v>215</v>
       </c>
@@ -4785,7 +4902,7 @@
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
     </row>
-    <row r="57" spans="1:27" ht="39.6">
+    <row r="57" spans="1:27" ht="26.4">
       <c r="A57" s="17" t="s">
         <v>496</v>
       </c>
@@ -5142,7 +5259,7 @@
       <c r="Z63" s="9"/>
       <c r="AA63" s="9"/>
     </row>
-    <row r="64" spans="1:27" ht="26.4">
+    <row r="64" spans="1:27" ht="13.2">
       <c r="A64" s="5" t="s">
         <v>276</v>
       </c>
@@ -5448,7 +5565,7 @@
       <c r="Z69" s="6"/>
       <c r="AA69" s="6"/>
     </row>
-    <row r="70" spans="1:27" ht="79.2">
+    <row r="70" spans="1:27" ht="52.8">
       <c r="A70" s="6" t="s">
         <v>304</v>
       </c>
@@ -5550,7 +5667,7 @@
       <c r="Z71" s="6"/>
       <c r="AA71" s="6"/>
     </row>
-    <row r="72" spans="1:27" ht="66.599999999999994" thickBot="1">
+    <row r="72" spans="1:27" ht="53.4" thickBot="1">
       <c r="A72" s="6" t="s">
         <v>306</v>
       </c>
@@ -5601,7 +5718,7 @@
       <c r="Z72" s="9"/>
       <c r="AA72" s="9"/>
     </row>
-    <row r="73" spans="1:27" ht="106.2" thickBot="1">
+    <row r="73" spans="1:27" ht="93" thickBot="1">
       <c r="A73" s="6" t="s">
         <v>311</v>
       </c>
@@ -5646,7 +5763,7 @@
       <c r="Z73" s="11"/>
       <c r="AA73" s="11"/>
     </row>
-    <row r="74" spans="1:27" ht="118.8">
+    <row r="74" spans="1:27" ht="105.6">
       <c r="A74" s="9" t="s">
         <v>318</v>
       </c>
@@ -5799,7 +5916,7 @@
       <c r="Z76" s="9"/>
       <c r="AA76" s="9"/>
     </row>
-    <row r="77" spans="1:27" ht="145.80000000000001" thickBot="1">
+    <row r="77" spans="1:27" ht="119.4" thickBot="1">
       <c r="A77" s="11" t="s">
         <v>354</v>
       </c>
@@ -6101,7 +6218,7 @@
       <c r="Z82" s="11"/>
       <c r="AA82" s="11"/>
     </row>
-    <row r="83" spans="1:27" ht="27" thickBot="1">
+    <row r="83" spans="1:27" ht="13.8" thickBot="1">
       <c r="A83" s="11" t="s">
         <v>368</v>
       </c>
@@ -6446,18 +6563,40 @@
       <c r="Z89" s="6"/>
       <c r="AA89" s="6"/>
     </row>
-    <row r="90" spans="1:27" ht="13.2">
-      <c r="A90" s="6"/>
-      <c r="B90" s="6"/>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="6"/>
-      <c r="H90" s="6"/>
-      <c r="I90" s="6"/>
-      <c r="J90" s="6"/>
-      <c r="K90" s="6"/>
+    <row r="90" spans="1:27" ht="27" thickBot="1">
+      <c r="A90" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I90" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J90" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="L90" s="6"/>
       <c r="M90" s="6"/>
       <c r="N90" s="6"/>
@@ -6475,18 +6614,40 @@
       <c r="Z90" s="6"/>
       <c r="AA90" s="6"/>
     </row>
-    <row r="91" spans="1:27" ht="13.2">
-      <c r="A91" s="6"/>
-      <c r="B91" s="6"/>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="6"/>
-      <c r="I91" s="6"/>
-      <c r="J91" s="6"/>
-      <c r="K91" s="6"/>
+    <row r="91" spans="1:27" ht="40.200000000000003" thickBot="1">
+      <c r="A91" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I91" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J91" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K91" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L91" s="6"/>
       <c r="M91" s="6"/>
       <c r="N91" s="6"/>
@@ -6504,18 +6665,40 @@
       <c r="Z91" s="6"/>
       <c r="AA91" s="6"/>
     </row>
-    <row r="92" spans="1:27" ht="13.2">
-      <c r="A92" s="6"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
-      <c r="J92" s="6"/>
-      <c r="K92" s="6"/>
+    <row r="92" spans="1:27" ht="27" thickBot="1">
+      <c r="A92" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F92" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H92" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I92" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J92" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K92" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L92" s="6"/>
       <c r="M92" s="6"/>
       <c r="N92" s="6"/>
@@ -6533,18 +6716,40 @@
       <c r="Z92" s="6"/>
       <c r="AA92" s="6"/>
     </row>
-    <row r="93" spans="1:27" ht="13.2">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="6"/>
-      <c r="G93" s="6"/>
-      <c r="H93" s="6"/>
-      <c r="I93" s="6"/>
-      <c r="J93" s="6"/>
-      <c r="K93" s="6"/>
+    <row r="93" spans="1:27" ht="40.200000000000003" thickBot="1">
+      <c r="A93" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H93" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I93" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J93" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K93" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L93" s="6"/>
       <c r="M93" s="6"/>
       <c r="N93" s="6"/>
@@ -6562,18 +6767,40 @@
       <c r="Z93" s="6"/>
       <c r="AA93" s="6"/>
     </row>
-    <row r="94" spans="1:27" ht="13.2">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6"/>
-      <c r="H94" s="6"/>
-      <c r="I94" s="6"/>
-      <c r="J94" s="6"/>
-      <c r="K94" s="6"/>
+    <row r="94" spans="1:27" ht="79.8" thickBot="1">
+      <c r="A94" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="F94" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I94" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J94" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K94" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L94" s="6"/>
       <c r="M94" s="6"/>
       <c r="N94" s="6"/>
@@ -6591,18 +6818,40 @@
       <c r="Z94" s="6"/>
       <c r="AA94" s="6"/>
     </row>
-    <row r="95" spans="1:27" ht="13.2">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
-      <c r="F95" s="6"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="6"/>
-      <c r="J95" s="6"/>
-      <c r="K95" s="6"/>
+    <row r="95" spans="1:27" ht="40.200000000000003" thickBot="1">
+      <c r="A95" s="19" t="s">
+        <v>523</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F95" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H95" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I95" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J95" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K95" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L95" s="6"/>
       <c r="M95" s="6"/>
       <c r="N95" s="6"/>
@@ -6620,18 +6869,40 @@
       <c r="Z95" s="6"/>
       <c r="AA95" s="6"/>
     </row>
-    <row r="96" spans="1:27" ht="13.2">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
-      <c r="H96" s="6"/>
-      <c r="I96" s="6"/>
-      <c r="J96" s="6"/>
-      <c r="K96" s="6"/>
+    <row r="96" spans="1:27" ht="27" thickBot="1">
+      <c r="A96" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="D96" s="21" t="s">
+        <v>528</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F96" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H96" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I96" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J96" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K96" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L96" s="6"/>
       <c r="M96" s="6"/>
       <c r="N96" s="6"/>
@@ -6649,18 +6920,28 @@
       <c r="Z96" s="6"/>
       <c r="AA96" s="6"/>
     </row>
-    <row r="97" spans="1:27" ht="13.2">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="6"/>
-      <c r="I97" s="6"/>
-      <c r="J97" s="6"/>
-      <c r="K97" s="6"/>
+    <row r="97" spans="1:27" ht="27" thickBot="1">
+      <c r="A97" s="19" t="s">
+        <v>529</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="D97" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L97" s="6"/>
       <c r="M97" s="6"/>
       <c r="N97" s="6"/>
@@ -6678,18 +6959,36 @@
       <c r="Z97" s="6"/>
       <c r="AA97" s="6"/>
     </row>
-    <row r="98" spans="1:27" ht="13.2">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="6"/>
-      <c r="J98" s="6"/>
-      <c r="K98" s="6"/>
+    <row r="98" spans="1:27" ht="40.200000000000003" thickBot="1">
+      <c r="A98" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="F98" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="G98" s="11"/>
+      <c r="H98" s="11"/>
+      <c r="I98" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="J98" s="21" t="s">
+        <v>538</v>
+      </c>
+      <c r="K98" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L98" s="6"/>
       <c r="M98" s="6"/>
       <c r="N98" s="6"/>
@@ -6707,18 +7006,40 @@
       <c r="Z98" s="6"/>
       <c r="AA98" s="6"/>
     </row>
-    <row r="99" spans="1:27" ht="13.2">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="6"/>
-      <c r="G99" s="6"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="6"/>
-      <c r="J99" s="6"/>
-      <c r="K99" s="6"/>
+    <row r="99" spans="1:27" ht="27" thickBot="1">
+      <c r="A99" s="19" t="s">
+        <v>539</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H99" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I99" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J99" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K99" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="L99" s="6"/>
       <c r="M99" s="6"/>
       <c r="N99" s="6"/>
@@ -33099,8 +33420,18 @@
     <hyperlink ref="B57" r:id="rId85"/>
     <hyperlink ref="B88" r:id="rId86"/>
     <hyperlink ref="B89" r:id="rId87"/>
+    <hyperlink ref="B90" r:id="rId88"/>
+    <hyperlink ref="B91" r:id="rId89"/>
+    <hyperlink ref="B92" r:id="rId90"/>
+    <hyperlink ref="B93" r:id="rId91"/>
+    <hyperlink ref="B94" r:id="rId92"/>
+    <hyperlink ref="B95" r:id="rId93"/>
+    <hyperlink ref="B96" r:id="rId94"/>
+    <hyperlink ref="B97" r:id="rId95"/>
+    <hyperlink ref="B98" r:id="rId96"/>
+    <hyperlink ref="B99" r:id="rId97"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId88"/>
+  <pageSetup orientation="portrait" r:id="rId98"/>
 </worksheet>
 </file>
</xml_diff>